<commit_message>
removed obsolete data files,visualised climate trends
</commit_message>
<xml_diff>
--- a/Data/Semi-prepared data/Predicted_Temperature.xlsx
+++ b/Data/Semi-prepared data/Predicted_Temperature.xlsx
@@ -56328,2858 +56328,2858 @@
     </row>
     <row r="470">
       <c r="A470" s="2" t="n">
-        <v>44926</v>
+        <v>44927</v>
       </c>
       <c r="B470" t="n">
-        <v>21.19255550201111</v>
+        <v>20.96255548759314</v>
       </c>
       <c r="C470" t="n">
-        <v>19.35898719040765</v>
+        <v>18.94341708133539</v>
       </c>
       <c r="D470" t="n">
-        <v>18.97409084254325</v>
+        <v>18.91718044821222</v>
       </c>
       <c r="E470" t="n">
-        <v>22.90742071191776</v>
+        <v>22.78318976147357</v>
       </c>
       <c r="F470" t="n">
-        <v>29.60998103161123</v>
+        <v>29.25749304019655</v>
       </c>
       <c r="G470" t="n">
-        <v>23.70268821425675</v>
+        <v>23.33528013971256</v>
       </c>
       <c r="H470" t="n">
-        <v>27.5383130552541</v>
+        <v>27.10805405185513</v>
       </c>
       <c r="I470" t="n">
-        <v>22.33277725571671</v>
+        <v>22.27507697911067</v>
       </c>
       <c r="J470" t="n">
-        <v>21.26387875816146</v>
+        <v>21.01446960937821</v>
       </c>
       <c r="K470" t="n">
-        <v>18.65328987342103</v>
+        <v>18.32641944791889</v>
       </c>
       <c r="L470" t="n">
-        <v>27.93933089441012</v>
+        <v>27.78088878870361</v>
       </c>
       <c r="M470" t="n">
-        <v>21.63971525481729</v>
+        <v>21.21104171779546</v>
       </c>
       <c r="N470" t="n">
-        <v>22.16358302251813</v>
+        <v>21.73998359506034</v>
       </c>
       <c r="O470" t="n">
-        <v>26.4483280541441</v>
+        <v>26.23092062550554</v>
       </c>
       <c r="P470" t="n">
-        <v>27.25078525924319</v>
+        <v>27.07793153446193</v>
       </c>
       <c r="Q470" t="n">
-        <v>19.62382141362336</v>
+        <v>19.43474027842277</v>
       </c>
       <c r="R470" t="n">
-        <v>28.46567064493493</v>
+        <v>28.20222700740116</v>
       </c>
       <c r="S470" t="n">
-        <v>21.2299867114187</v>
+        <v>21.14906917350029</v>
       </c>
       <c r="T470" t="n">
-        <v>23.21873017114485</v>
+        <v>23.14385797631063</v>
       </c>
       <c r="U470" t="n">
-        <v>27.41000332625525</v>
+        <v>26.85619280050139</v>
       </c>
       <c r="V470" t="n">
-        <v>29.21660408651758</v>
+        <v>28.46888527882685</v>
       </c>
       <c r="W470" t="n">
-        <v>22.16718109046534</v>
+        <v>21.91209847154901</v>
       </c>
       <c r="X470" t="n">
-        <v>18.92564068788858</v>
+        <v>18.77468029999739</v>
       </c>
       <c r="Y470" t="n">
-        <v>20.16510395477945</v>
+        <v>20.05565890417351</v>
       </c>
       <c r="Z470" t="n">
-        <v>16.47537236754575</v>
+        <v>16.22317259543951</v>
       </c>
       <c r="AA470" t="n">
-        <v>18.90135487562752</v>
+        <v>18.69128124225172</v>
       </c>
       <c r="AB470" t="n">
-        <v>20.07796457729193</v>
+        <v>19.7681306395331</v>
       </c>
       <c r="AC470" t="n">
-        <v>16.89716710998682</v>
+        <v>16.63463790800056</v>
       </c>
       <c r="AD470" t="n">
-        <v>17.52397568315113</v>
+        <v>17.36388718661217</v>
       </c>
       <c r="AE470" t="n">
-        <v>24.87549693913805</v>
+        <v>24.53842946374125</v>
       </c>
       <c r="AF470" t="n">
-        <v>23.86452619202761</v>
+        <v>23.49640161836479</v>
       </c>
       <c r="AG470" t="n">
-        <v>24.83068251508293</v>
+        <v>24.69498192769291</v>
       </c>
       <c r="AH470" t="n">
-        <v>29.39583143272619</v>
+        <v>29.04538287999998</v>
       </c>
       <c r="AI470" t="n">
-        <v>21.45478966894588</v>
+        <v>21.28999971685973</v>
       </c>
       <c r="AJ470" t="n">
-        <v>29.0511594231472</v>
+        <v>28.39549692581823</v>
       </c>
       <c r="AK470" t="n">
-        <v>19.00801071141566</v>
+        <v>18.86652750619175</v>
       </c>
       <c r="AL470" t="n">
-        <v>29.17242379864654</v>
+        <v>28.69085777956798</v>
       </c>
       <c r="AM470" t="n">
-        <v>24.02071630151246</v>
+        <v>23.70671046675572</v>
       </c>
     </row>
     <row r="471">
       <c r="A471" s="2" t="n">
-        <v>44957</v>
+        <v>44958</v>
       </c>
       <c r="B471" t="n">
-        <v>22.55216428957127</v>
+        <v>22.12479110147683</v>
       </c>
       <c r="C471" t="n">
-        <v>20.35502492463426</v>
+        <v>19.78121495223845</v>
       </c>
       <c r="D471" t="n">
-        <v>20.40257020438887</v>
+        <v>20.16272076966011</v>
       </c>
       <c r="E471" t="n">
-        <v>24.2610231880326</v>
+        <v>23.94887491942362</v>
       </c>
       <c r="F471" t="n">
-        <v>30.41750984242277</v>
+        <v>30.20098454012395</v>
       </c>
       <c r="G471" t="n">
-        <v>24.7851475792963</v>
+        <v>24.13508749750307</v>
       </c>
       <c r="H471" t="n">
-        <v>28.65034774345392</v>
+        <v>28.37207656207445</v>
       </c>
       <c r="I471" t="n">
-        <v>23.75301324575836</v>
+        <v>23.23073497296063</v>
       </c>
       <c r="J471" t="n">
-        <v>22.42211535676671</v>
+        <v>22.0743494499631</v>
       </c>
       <c r="K471" t="n">
-        <v>19.68864669803464</v>
+        <v>19.26111590591806</v>
       </c>
       <c r="L471" t="n">
-        <v>28.40952499671667</v>
+        <v>28.31726772719394</v>
       </c>
       <c r="M471" t="n">
-        <v>22.68666519002102</v>
+        <v>22.05821218791153</v>
       </c>
       <c r="N471" t="n">
-        <v>23.23452778701496</v>
+        <v>22.6631191382383</v>
       </c>
       <c r="O471" t="n">
-        <v>27.58971418764244</v>
+        <v>27.30159656679669</v>
       </c>
       <c r="P471" t="n">
-        <v>27.73087740061196</v>
+        <v>27.63216049123688</v>
       </c>
       <c r="Q471" t="n">
-        <v>20.90816599621106</v>
+        <v>20.57499589964359</v>
       </c>
       <c r="R471" t="n">
-        <v>28.70488377875902</v>
+        <v>28.57163438552661</v>
       </c>
       <c r="S471" t="n">
-        <v>22.72422989864241</v>
+        <v>22.28777446014166</v>
       </c>
       <c r="T471" t="n">
-        <v>24.55443017869979</v>
+        <v>24.16935165420244</v>
       </c>
       <c r="U471" t="n">
-        <v>28.54212203297396</v>
+        <v>28.30681977479867</v>
       </c>
       <c r="V471" t="n">
-        <v>30.3125815445446</v>
+        <v>29.68412365014132</v>
       </c>
       <c r="W471" t="n">
-        <v>23.30717229783054</v>
+        <v>23.05662934927387</v>
       </c>
       <c r="X471" t="n">
-        <v>20.18849114536645</v>
+        <v>19.83230836128961</v>
       </c>
       <c r="Y471" t="n">
-        <v>21.62405211638217</v>
+        <v>21.13605702450614</v>
       </c>
       <c r="Z471" t="n">
-        <v>17.56229263360108</v>
+        <v>17.12036606621662</v>
       </c>
       <c r="AA471" t="n">
-        <v>20.15865050908105</v>
+        <v>19.80559196773253</v>
       </c>
       <c r="AB471" t="n">
-        <v>21.22750748410043</v>
+        <v>20.57307551264472</v>
       </c>
       <c r="AC471" t="n">
-        <v>17.933584722246</v>
+        <v>17.57179070020706</v>
       </c>
       <c r="AD471" t="n">
-        <v>18.70805141707084</v>
+        <v>18.40766424636554</v>
       </c>
       <c r="AE471" t="n">
-        <v>26.06356209242146</v>
+        <v>25.70131737078386</v>
       </c>
       <c r="AF471" t="n">
-        <v>24.84503893108629</v>
+        <v>24.36077672455952</v>
       </c>
       <c r="AG471" t="n">
-        <v>25.72502506090104</v>
+        <v>25.48534829127701</v>
       </c>
       <c r="AH471" t="n">
-        <v>30.20617346192018</v>
+        <v>29.98960645818359</v>
       </c>
       <c r="AI471" t="n">
-        <v>22.7018464520343</v>
+        <v>22.44003045690638</v>
       </c>
       <c r="AJ471" t="n">
-        <v>30.23858107208752</v>
+        <v>29.62666165987773</v>
       </c>
       <c r="AK471" t="n">
-        <v>20.55951489133128</v>
+        <v>20.18022787945774</v>
       </c>
       <c r="AL471" t="n">
-        <v>30.48282720588488</v>
+        <v>30.0681370229986</v>
       </c>
       <c r="AM471" t="n">
-        <v>25.38068753609241</v>
+        <v>24.96263497013021</v>
       </c>
     </row>
     <row r="472">
       <c r="A472" s="2" t="n">
-        <v>44985</v>
+        <v>44986</v>
       </c>
       <c r="B472" t="n">
-        <v>21.85718083856325</v>
+        <v>22.46359857980305</v>
       </c>
       <c r="C472" t="n">
-        <v>18.67485409341979</v>
+        <v>19.62695365234</v>
       </c>
       <c r="D472" t="n">
-        <v>20.24611237235744</v>
+        <v>20.63372748600807</v>
       </c>
       <c r="E472" t="n">
-        <v>23.46390284690938</v>
+        <v>24.05104802593572</v>
       </c>
       <c r="F472" t="n">
-        <v>30.07320359744503</v>
+        <v>30.37941964625546</v>
       </c>
       <c r="G472" t="n">
-        <v>23.11690564414292</v>
+        <v>23.83612705755799</v>
       </c>
       <c r="H472" t="n">
-        <v>28.15105061044117</v>
+        <v>28.73985689234787</v>
       </c>
       <c r="I472" t="n">
-        <v>22.26823343967825</v>
+        <v>22.99630320650871</v>
       </c>
       <c r="J472" t="n">
-        <v>21.74737835635129</v>
+        <v>22.29217734506312</v>
       </c>
       <c r="K472" t="n">
-        <v>18.73565091216171</v>
+        <v>19.4759568780823</v>
       </c>
       <c r="L472" t="n">
-        <v>27.94404970933897</v>
+        <v>28.26538080771539</v>
       </c>
       <c r="M472" t="n">
-        <v>20.94610890106744</v>
+        <v>21.84713552848698</v>
       </c>
       <c r="N472" t="n">
-        <v>21.77629790099604</v>
+        <v>22.58371554975386</v>
       </c>
       <c r="O472" t="n">
-        <v>26.576369256455</v>
+        <v>27.15044818856117</v>
       </c>
       <c r="P472" t="n">
-        <v>26.90977805510743</v>
+        <v>27.24440825973461</v>
       </c>
       <c r="Q472" t="n">
-        <v>20.42943690932237</v>
+        <v>20.98041342837299</v>
       </c>
       <c r="R472" t="n">
-        <v>28.78946202165462</v>
+        <v>29.03466069171466</v>
       </c>
       <c r="S472" t="n">
-        <v>21.60173738374406</v>
+        <v>22.30518561020181</v>
       </c>
       <c r="T472" t="n">
-        <v>23.35204946227089</v>
+        <v>24.055207063974</v>
       </c>
       <c r="U472" t="n">
-        <v>28.60202149590184</v>
+        <v>28.96656884742918</v>
       </c>
       <c r="V472" t="n">
-        <v>28.3434465252172</v>
+        <v>29.4077300532088</v>
       </c>
       <c r="W472" t="n">
-        <v>22.91015003876414</v>
+        <v>23.43513695128414</v>
       </c>
       <c r="X472" t="n">
-        <v>19.21806980331691</v>
+        <v>19.8761341536851</v>
       </c>
       <c r="Y472" t="n">
-        <v>20.30315416662464</v>
+        <v>21.02915657537381</v>
       </c>
       <c r="Z472" t="n">
-        <v>16.43749096840016</v>
+        <v>17.21401770717549</v>
       </c>
       <c r="AA472" t="n">
-        <v>19.59750837725337</v>
+        <v>20.20879206405426</v>
       </c>
       <c r="AB472" t="n">
-        <v>19.22409025956527</v>
+        <v>20.19919769806006</v>
       </c>
       <c r="AC472" t="n">
-        <v>17.08568695155437</v>
+        <v>17.80711751162834</v>
       </c>
       <c r="AD472" t="n">
-        <v>18.05181408312121</v>
+        <v>18.61563709997241</v>
       </c>
       <c r="AE472" t="n">
-        <v>25.50266693243053</v>
+        <v>26.06390108916727</v>
       </c>
       <c r="AF472" t="n">
-        <v>23.6162197254103</v>
+        <v>24.20349598215145</v>
       </c>
       <c r="AG472" t="n">
-        <v>24.56133867979964</v>
+        <v>25.0983309115607</v>
       </c>
       <c r="AH472" t="n">
-        <v>29.38369261719181</v>
+        <v>29.76706453414388</v>
       </c>
       <c r="AI472" t="n">
-        <v>22.16480572848753</v>
+        <v>22.69897831682236</v>
       </c>
       <c r="AJ472" t="n">
-        <v>28.68685644607914</v>
+        <v>29.5453141934012</v>
       </c>
       <c r="AK472" t="n">
-        <v>20.03447179000232</v>
+        <v>20.61396181243006</v>
       </c>
       <c r="AL472" t="n">
-        <v>29.64526625589235</v>
+        <v>30.22426914694116</v>
       </c>
       <c r="AM472" t="n">
-        <v>24.63247048835671</v>
+        <v>25.193849896556</v>
       </c>
     </row>
     <row r="473">
       <c r="A473" s="2" t="n">
-        <v>45016</v>
+        <v>45017</v>
       </c>
       <c r="B473" t="n">
-        <v>22.27815599926079</v>
+        <v>22.1012720180474</v>
       </c>
       <c r="C473" t="n">
-        <v>19.34802826289732</v>
+        <v>18.91066787134007</v>
       </c>
       <c r="D473" t="n">
-        <v>20.37941325261724</v>
+        <v>19.99876147542864</v>
       </c>
       <c r="E473" t="n">
-        <v>23.80465311729328</v>
+        <v>23.51298718174491</v>
       </c>
       <c r="F473" t="n">
-        <v>29.39530919335424</v>
+        <v>29.14094622962384</v>
       </c>
       <c r="G473" t="n">
-        <v>23.41608680730939</v>
+        <v>23.11756738269907</v>
       </c>
       <c r="H473" t="n">
-        <v>28.11438256718302</v>
+        <v>27.94147390466113</v>
       </c>
       <c r="I473" t="n">
-        <v>22.79198167392174</v>
+        <v>22.35666385408834</v>
       </c>
       <c r="J473" t="n">
-        <v>21.95207919171857</v>
+        <v>21.54493497072175</v>
       </c>
       <c r="K473" t="n">
-        <v>19.32634162441704</v>
+        <v>18.95759592403617</v>
       </c>
       <c r="L473" t="n">
-        <v>27.70261224716566</v>
+        <v>27.43788795487206</v>
       </c>
       <c r="M473" t="n">
-        <v>21.54578893811058</v>
+        <v>21.11896281078782</v>
       </c>
       <c r="N473" t="n">
-        <v>22.1946787989512</v>
+        <v>21.81418352766321</v>
       </c>
       <c r="O473" t="n">
-        <v>26.72236240501507</v>
+        <v>26.31504629267054</v>
       </c>
       <c r="P473" t="n">
-        <v>26.37290950700521</v>
+        <v>26.07196863899549</v>
       </c>
       <c r="Q473" t="n">
-        <v>20.8626767121394</v>
+        <v>20.84279158548864</v>
       </c>
       <c r="R473" t="n">
-        <v>28.79803660651677</v>
+        <v>28.72843516529645</v>
       </c>
       <c r="S473" t="n">
-        <v>22.08051192451203</v>
+        <v>21.7887742056491</v>
       </c>
       <c r="T473" t="n">
-        <v>23.88094546609119</v>
+        <v>23.48080508303006</v>
       </c>
       <c r="U473" t="n">
-        <v>27.50691669265698</v>
+        <v>27.3875522283671</v>
       </c>
       <c r="V473" t="n">
-        <v>28.4021946374739</v>
+        <v>28.28320128937454</v>
       </c>
       <c r="W473" t="n">
-        <v>23.17976520999104</v>
+        <v>23.05363543635567</v>
       </c>
       <c r="X473" t="n">
-        <v>19.64523822797585</v>
+        <v>19.43382004652494</v>
       </c>
       <c r="Y473" t="n">
-        <v>20.72264240802575</v>
+        <v>20.43941966750018</v>
       </c>
       <c r="Z473" t="n">
-        <v>17.15268401295186</v>
+        <v>16.83371291458706</v>
       </c>
       <c r="AA473" t="n">
-        <v>20.08283322319603</v>
+        <v>19.748552254111</v>
       </c>
       <c r="AB473" t="n">
-        <v>19.93028257179676</v>
+        <v>19.45563508499092</v>
       </c>
       <c r="AC473" t="n">
-        <v>17.85187197944923</v>
+        <v>17.52986140260525</v>
       </c>
       <c r="AD473" t="n">
-        <v>18.36383804196117</v>
+        <v>18.28225684996224</v>
       </c>
       <c r="AE473" t="n">
-        <v>25.68539180165664</v>
+        <v>25.70545475809722</v>
       </c>
       <c r="AF473" t="n">
-        <v>23.67730284155394</v>
+        <v>23.30097891564328</v>
       </c>
       <c r="AG473" t="n">
-        <v>24.44855056296261</v>
+        <v>24.06109309167971</v>
       </c>
       <c r="AH473" t="n">
-        <v>28.72453339280264</v>
+        <v>28.39645254879903</v>
       </c>
       <c r="AI473" t="n">
-        <v>22.47170556113929</v>
+        <v>22.27033428589503</v>
       </c>
       <c r="AJ473" t="n">
-        <v>28.75672578022634</v>
+        <v>28.67034300723613</v>
       </c>
       <c r="AK473" t="n">
-        <v>20.41142639232848</v>
+        <v>20.11499834919289</v>
       </c>
       <c r="AL473" t="n">
-        <v>28.92801955107548</v>
+        <v>28.68185056035242</v>
       </c>
       <c r="AM473" t="n">
-        <v>24.67879709744415</v>
+        <v>24.5580498063125</v>
       </c>
     </row>
     <row r="474">
       <c r="A474" s="2" t="n">
-        <v>45046</v>
+        <v>45047</v>
       </c>
       <c r="B474" t="n">
-        <v>21.29792872465971</v>
+        <v>21.2248679065037</v>
       </c>
       <c r="C474" t="n">
-        <v>17.7495042108634</v>
+        <v>17.7217815267553</v>
       </c>
       <c r="D474" t="n">
-        <v>18.78164423898918</v>
+        <v>18.79969718577219</v>
       </c>
       <c r="E474" t="n">
-        <v>22.35921282489345</v>
+        <v>22.38667332780218</v>
       </c>
       <c r="F474" t="n">
-        <v>26.92343583225682</v>
+        <v>27.19712196323568</v>
       </c>
       <c r="G474" t="n">
-        <v>22.25517291424577</v>
+        <v>22.31680581317837</v>
       </c>
       <c r="H474" t="n">
-        <v>27.05040793211113</v>
+        <v>27.04958177708003</v>
       </c>
       <c r="I474" t="n">
-        <v>20.82421679815817</v>
+        <v>20.90149475821882</v>
       </c>
       <c r="J474" t="n">
-        <v>20.43020262588304</v>
+        <v>20.44015144764253</v>
       </c>
       <c r="K474" t="n">
-        <v>17.99444567193992</v>
+        <v>17.97297923795676</v>
       </c>
       <c r="L474" t="n">
-        <v>25.80625498096038</v>
+        <v>25.91030624586456</v>
       </c>
       <c r="M474" t="n">
-        <v>20.08773468550715</v>
+        <v>20.07749582419862</v>
       </c>
       <c r="N474" t="n">
-        <v>20.90621604252188</v>
+        <v>20.87296859008885</v>
       </c>
       <c r="O474" t="n">
-        <v>24.86700205125711</v>
+        <v>25.04110424586304</v>
       </c>
       <c r="P474" t="n">
-        <v>24.42143739527899</v>
+        <v>24.49833866617144</v>
       </c>
       <c r="Q474" t="n">
-        <v>20.53522238965334</v>
+        <v>20.34391398066566</v>
       </c>
       <c r="R474" t="n">
-        <v>27.18650173871052</v>
+        <v>27.27807454614244</v>
       </c>
       <c r="S474" t="n">
-        <v>20.50738385148381</v>
+        <v>20.43462428540758</v>
       </c>
       <c r="T474" t="n">
-        <v>22.08427663472448</v>
+        <v>22.09495799167808</v>
       </c>
       <c r="U474" t="n">
-        <v>26.12471717831608</v>
+        <v>26.0950707301971</v>
       </c>
       <c r="V474" t="n">
-        <v>27.8245653543182</v>
+        <v>27.63927888911973</v>
       </c>
       <c r="W474" t="n">
-        <v>22.43481409609228</v>
+        <v>22.37998955357131</v>
       </c>
       <c r="X474" t="n">
-        <v>18.32419234949842</v>
+        <v>18.2484403625434</v>
       </c>
       <c r="Y474" t="n">
-        <v>19.1174866667247</v>
+        <v>19.07111563398931</v>
       </c>
       <c r="Z474" t="n">
-        <v>15.69157617151719</v>
+        <v>15.69098671779848</v>
       </c>
       <c r="AA474" t="n">
-        <v>18.75393324791986</v>
+        <v>18.71279976009968</v>
       </c>
       <c r="AB474" t="n">
-        <v>18.08591491656434</v>
+        <v>18.05772534514318</v>
       </c>
       <c r="AC474" t="n">
-        <v>16.48641931917586</v>
+        <v>16.47808976778314</v>
       </c>
       <c r="AD474" t="n">
-        <v>17.55502102165516</v>
+        <v>17.4241147073419</v>
       </c>
       <c r="AE474" t="n">
-        <v>25.4593276945923</v>
+        <v>25.35820004665735</v>
       </c>
       <c r="AF474" t="n">
-        <v>22.27527425282504</v>
+        <v>22.36537773529686</v>
       </c>
       <c r="AG474" t="n">
-        <v>22.26163778379124</v>
+        <v>22.41065930949615</v>
       </c>
       <c r="AH474" t="n">
-        <v>26.40535831263061</v>
+        <v>26.68183932770066</v>
       </c>
       <c r="AI474" t="n">
-        <v>21.39295881981115</v>
+        <v>21.38533795205283</v>
       </c>
       <c r="AJ474" t="n">
-        <v>28.31826893522363</v>
+        <v>28.10395422307477</v>
       </c>
       <c r="AK474" t="n">
-        <v>19.03984935429472</v>
+        <v>19.00016517025598</v>
       </c>
       <c r="AL474" t="n">
-        <v>27.14972096851663</v>
+        <v>27.17592642812789</v>
       </c>
       <c r="AM474" t="n">
-        <v>23.83130456615856</v>
+        <v>23.66902331985805</v>
       </c>
     </row>
     <row r="475">
       <c r="A475" s="2" t="n">
-        <v>45077</v>
+        <v>45078</v>
       </c>
       <c r="B475" t="n">
-        <v>20.43585182322434</v>
+        <v>20.42670501305767</v>
       </c>
       <c r="C475" t="n">
-        <v>16.99725271346711</v>
+        <v>16.9102795701402</v>
       </c>
       <c r="D475" t="n">
-        <v>17.72996377892115</v>
+        <v>17.89119210287736</v>
       </c>
       <c r="E475" t="n">
-        <v>21.59256524955742</v>
+        <v>21.45206531717214</v>
       </c>
       <c r="F475" t="n">
-        <v>26.361601235022</v>
+        <v>26.26096074905064</v>
       </c>
       <c r="G475" t="n">
-        <v>21.81693874874084</v>
+        <v>21.95737119496222</v>
       </c>
       <c r="H475" t="n">
-        <v>26.29069847949464</v>
+        <v>26.21914993976968</v>
       </c>
       <c r="I475" t="n">
-        <v>20.10892648736728</v>
+        <v>20.1251726549533</v>
       </c>
       <c r="J475" t="n">
-        <v>19.36347641576859</v>
+        <v>19.5765024038889</v>
       </c>
       <c r="K475" t="n">
-        <v>17.15311282356136</v>
+        <v>17.15483615906266</v>
       </c>
       <c r="L475" t="n">
-        <v>24.76117230972476</v>
+        <v>24.75927352174429</v>
       </c>
       <c r="M475" t="n">
-        <v>19.35659081877181</v>
+        <v>19.43284692301409</v>
       </c>
       <c r="N475" t="n">
-        <v>19.93983155114705</v>
+        <v>20.12361884841277</v>
       </c>
       <c r="O475" t="n">
-        <v>24.29320809697604</v>
+        <v>24.21216102618965</v>
       </c>
       <c r="P475" t="n">
-        <v>23.17256458461752</v>
+        <v>23.24661447535992</v>
       </c>
       <c r="Q475" t="n">
-        <v>19.79084184408399</v>
+        <v>19.64164744291755</v>
       </c>
       <c r="R475" t="n">
-        <v>26.29258296540268</v>
+        <v>26.14769371317098</v>
       </c>
       <c r="S475" t="n">
-        <v>19.70169786325566</v>
+        <v>19.58347820441352</v>
       </c>
       <c r="T475" t="n">
-        <v>21.27888871127266</v>
+        <v>21.18933206244574</v>
       </c>
       <c r="U475" t="n">
-        <v>25.37541588548278</v>
+        <v>25.50702587883671</v>
       </c>
       <c r="V475" t="n">
-        <v>27.04973877397439</v>
+        <v>26.94026819907387</v>
       </c>
       <c r="W475" t="n">
-        <v>21.81250560806028</v>
+        <v>21.69631340160895</v>
       </c>
       <c r="X475" t="n">
-        <v>17.64678736308003</v>
+        <v>17.41250189240072</v>
       </c>
       <c r="Y475" t="n">
-        <v>18.47744656849722</v>
+        <v>18.37426284468925</v>
       </c>
       <c r="Z475" t="n">
-        <v>15.15306699924653</v>
+        <v>14.90979615057354</v>
       </c>
       <c r="AA475" t="n">
-        <v>17.8019628565445</v>
+        <v>17.83576230203594</v>
       </c>
       <c r="AB475" t="n">
-        <v>17.32095435699374</v>
+        <v>17.26439507975673</v>
       </c>
       <c r="AC475" t="n">
-        <v>16.01147378065239</v>
+        <v>15.76529936099715</v>
       </c>
       <c r="AD475" t="n">
-        <v>16.91646436709663</v>
+        <v>16.63992161624755</v>
       </c>
       <c r="AE475" t="n">
-        <v>24.68836080086742</v>
+        <v>24.56940785750129</v>
       </c>
       <c r="AF475" t="n">
-        <v>21.58407011498398</v>
+        <v>21.81938393602987</v>
       </c>
       <c r="AG475" t="n">
-        <v>21.34451511450224</v>
+        <v>21.27163756677774</v>
       </c>
       <c r="AH475" t="n">
-        <v>25.91333492328587</v>
+        <v>25.86305656632063</v>
       </c>
       <c r="AI475" t="n">
-        <v>20.75019031095585</v>
+        <v>20.59927686153897</v>
       </c>
       <c r="AJ475" t="n">
-        <v>27.28452766219472</v>
+        <v>27.33681698130986</v>
       </c>
       <c r="AK475" t="n">
-        <v>18.13082522676346</v>
+        <v>18.16064770511035</v>
       </c>
       <c r="AL475" t="n">
-        <v>26.29231996864299</v>
+        <v>26.37129268957138</v>
       </c>
       <c r="AM475" t="n">
-        <v>22.59227685592473</v>
+        <v>22.69373004054869</v>
       </c>
     </row>
     <row r="476">
       <c r="A476" s="2" t="n">
-        <v>45107</v>
+        <v>45108</v>
       </c>
       <c r="B476" t="n">
-        <v>19.78999262809673</v>
+        <v>19.70504375973167</v>
       </c>
       <c r="C476" t="n">
-        <v>16.51663410276978</v>
+        <v>16.52086529735045</v>
       </c>
       <c r="D476" t="n">
-        <v>17.59139528102286</v>
+        <v>17.47044319801788</v>
       </c>
       <c r="E476" t="n">
-        <v>20.87274991469421</v>
+        <v>20.82027972928043</v>
       </c>
       <c r="F476" t="n">
-        <v>25.88890117137759</v>
+        <v>25.76739358582866</v>
       </c>
       <c r="G476" t="n">
-        <v>22.348238294306</v>
+        <v>22.21081775561609</v>
       </c>
       <c r="H476" t="n">
-        <v>25.80316066424263</v>
+        <v>25.66777991472038</v>
       </c>
       <c r="I476" t="n">
-        <v>20.07444219427171</v>
+        <v>19.95426915131695</v>
       </c>
       <c r="J476" t="n">
-        <v>19.46647153504093</v>
+        <v>19.31292084147349</v>
       </c>
       <c r="K476" t="n">
-        <v>16.79778083819039</v>
+        <v>16.72672509411304</v>
       </c>
       <c r="L476" t="n">
-        <v>24.46963415046982</v>
+        <v>24.31314072134769</v>
       </c>
       <c r="M476" t="n">
-        <v>19.49688892160017</v>
+        <v>19.43920862626309</v>
       </c>
       <c r="N476" t="n">
-        <v>20.1833644527488</v>
+        <v>20.03322945871772</v>
       </c>
       <c r="O476" t="n">
-        <v>23.71007539785015</v>
+        <v>23.59726761716198</v>
       </c>
       <c r="P476" t="n">
-        <v>23.03964721888864</v>
+        <v>22.87559262508775</v>
       </c>
       <c r="Q476" t="n">
-        <v>18.88612329604673</v>
+        <v>18.90910576178246</v>
       </c>
       <c r="R476" t="n">
-        <v>25.49776405378428</v>
+        <v>25.44539665294528</v>
       </c>
       <c r="S476" t="n">
-        <v>19.28084093765547</v>
+        <v>19.24317072982369</v>
       </c>
       <c r="T476" t="n">
-        <v>20.84162718240772</v>
+        <v>20.80672975320541</v>
       </c>
       <c r="U476" t="n">
-        <v>25.21416572208372</v>
+        <v>25.15407635949301</v>
       </c>
       <c r="V476" t="n">
-        <v>26.67171576599702</v>
+        <v>26.54782294902991</v>
       </c>
       <c r="W476" t="n">
-        <v>21.22608472914284</v>
+        <v>21.1456377451662</v>
       </c>
       <c r="X476" t="n">
-        <v>16.84158783384568</v>
+        <v>16.85433942550434</v>
       </c>
       <c r="Y476" t="n">
-        <v>18.22730086501792</v>
+        <v>18.14064908278271</v>
       </c>
       <c r="Z476" t="n">
-        <v>14.18868845727984</v>
+        <v>14.19878388484584</v>
       </c>
       <c r="AA476" t="n">
-        <v>17.424131708458</v>
+        <v>17.3433748529491</v>
       </c>
       <c r="AB476" t="n">
-        <v>16.97968261406739</v>
+        <v>16.99595517695157</v>
       </c>
       <c r="AC476" t="n">
-        <v>14.90556202883423</v>
+        <v>14.9598742127607</v>
       </c>
       <c r="AD476" t="n">
-        <v>15.88159980858252</v>
+        <v>15.93665932020275</v>
       </c>
       <c r="AE476" t="n">
-        <v>24.06279661792969</v>
+        <v>23.98508616180783</v>
       </c>
       <c r="AF476" t="n">
-        <v>22.04417979349071</v>
+        <v>21.85637834626207</v>
       </c>
       <c r="AG476" t="n">
-        <v>20.90474637023524</v>
+        <v>20.78268719092192</v>
       </c>
       <c r="AH476" t="n">
-        <v>25.56572457860812</v>
+        <v>25.39858005315718</v>
       </c>
       <c r="AI476" t="n">
-        <v>20.02969314533902</v>
+        <v>19.97329967783239</v>
       </c>
       <c r="AJ476" t="n">
-        <v>26.85363106498331</v>
+        <v>26.82328754641044</v>
       </c>
       <c r="AK476" t="n">
-        <v>17.71722734772205</v>
+        <v>17.62740644268204</v>
       </c>
       <c r="AL476" t="n">
-        <v>26.12098728820382</v>
+        <v>26.031608954996</v>
       </c>
       <c r="AM476" t="n">
-        <v>22.19181092707354</v>
+        <v>22.09667073289573</v>
       </c>
     </row>
     <row r="477">
       <c r="A477" s="2" t="n">
-        <v>45138</v>
+        <v>45139</v>
       </c>
       <c r="B477" t="n">
-        <v>19.86975127744496</v>
+        <v>19.89381089614971</v>
       </c>
       <c r="C477" t="n">
-        <v>16.97364861684255</v>
+        <v>17.10521233783632</v>
       </c>
       <c r="D477" t="n">
-        <v>17.61329650249888</v>
+        <v>17.74600504381406</v>
       </c>
       <c r="E477" t="n">
-        <v>21.10281910453772</v>
+        <v>21.18252199579791</v>
       </c>
       <c r="F477" t="n">
-        <v>26.12950163143914</v>
+        <v>26.15958403826502</v>
       </c>
       <c r="G477" t="n">
-        <v>22.67080368720476</v>
+        <v>22.79555209908084</v>
       </c>
       <c r="H477" t="n">
-        <v>25.95665154424919</v>
+        <v>25.99951489375694</v>
       </c>
       <c r="I477" t="n">
-        <v>20.55509714761758</v>
+        <v>20.627227513797</v>
       </c>
       <c r="J477" t="n">
-        <v>19.50380476005085</v>
+        <v>19.63193176541498</v>
       </c>
       <c r="K477" t="n">
-        <v>16.93897208379306</v>
+        <v>17.07368736993971</v>
       </c>
       <c r="L477" t="n">
-        <v>24.53342556630343</v>
+        <v>24.49563181667197</v>
       </c>
       <c r="M477" t="n">
-        <v>19.93197561716891</v>
+        <v>20.07420862441888</v>
       </c>
       <c r="N477" t="n">
-        <v>20.32713462326855</v>
+        <v>20.45461572449362</v>
       </c>
       <c r="O477" t="n">
-        <v>23.87207445880892</v>
+        <v>23.89579651720932</v>
       </c>
       <c r="P477" t="n">
-        <v>23.27994848542292</v>
+        <v>23.20858913596359</v>
       </c>
       <c r="Q477" t="n">
-        <v>19.05093060170624</v>
+        <v>19.12458386705445</v>
       </c>
       <c r="R477" t="n">
-        <v>25.48634689236366</v>
+        <v>25.48721781714159</v>
       </c>
       <c r="S477" t="n">
-        <v>19.5514228885502</v>
+        <v>19.7056186869454</v>
       </c>
       <c r="T477" t="n">
-        <v>21.1183737237982</v>
+        <v>21.19842169729995</v>
       </c>
       <c r="U477" t="n">
-        <v>25.6105292720989</v>
+        <v>25.64106465089825</v>
       </c>
       <c r="V477" t="n">
-        <v>27.08538464494254</v>
+        <v>27.06650369256074</v>
       </c>
       <c r="W477" t="n">
-        <v>21.34219516329484</v>
+        <v>21.44610095531415</v>
       </c>
       <c r="X477" t="n">
-        <v>17.16079050516275</v>
+        <v>17.29125910039242</v>
       </c>
       <c r="Y477" t="n">
-        <v>18.5245503448832</v>
+        <v>18.68635055170487</v>
       </c>
       <c r="Z477" t="n">
-        <v>14.40258086601455</v>
+        <v>14.54313611526392</v>
       </c>
       <c r="AA477" t="n">
-        <v>17.44591344314727</v>
+        <v>17.58878579653104</v>
       </c>
       <c r="AB477" t="n">
-        <v>17.69854508522598</v>
+        <v>17.80846959609689</v>
       </c>
       <c r="AC477" t="n">
-        <v>15.04038438755548</v>
+        <v>15.17282213187383</v>
       </c>
       <c r="AD477" t="n">
-        <v>16.08377306365018</v>
+        <v>16.21464679722052</v>
       </c>
       <c r="AE477" t="n">
-        <v>24.41477398390917</v>
+        <v>24.37911805003716</v>
       </c>
       <c r="AF477" t="n">
-        <v>22.11643564584197</v>
+        <v>22.22747931336088</v>
       </c>
       <c r="AG477" t="n">
-        <v>21.30451328173816</v>
+        <v>21.24402618289913</v>
       </c>
       <c r="AH477" t="n">
-        <v>25.7657423228991</v>
+        <v>25.73116136292813</v>
       </c>
       <c r="AI477" t="n">
-        <v>20.18524731192478</v>
+        <v>20.2776289462245</v>
       </c>
       <c r="AJ477" t="n">
-        <v>27.5191432590356</v>
+        <v>27.42435970622725</v>
       </c>
       <c r="AK477" t="n">
-        <v>17.71827216489276</v>
+        <v>17.83204917299556</v>
       </c>
       <c r="AL477" t="n">
-        <v>26.5328662974267</v>
+        <v>26.56276997390855</v>
       </c>
       <c r="AM477" t="n">
-        <v>22.45483095421905</v>
+        <v>22.45550459295788</v>
       </c>
     </row>
     <row r="478">
       <c r="A478" s="2" t="n">
-        <v>45169</v>
+        <v>45170</v>
       </c>
       <c r="B478" t="n">
-        <v>20.93592082000568</v>
+        <v>21.00302144687271</v>
       </c>
       <c r="C478" t="n">
-        <v>18.1667265600697</v>
+        <v>18.12872195384061</v>
       </c>
       <c r="D478" t="n">
-        <v>18.60411516404839</v>
+        <v>18.52586259115044</v>
       </c>
       <c r="E478" t="n">
-        <v>22.3401301338545</v>
+        <v>22.39849399765681</v>
       </c>
       <c r="F478" t="n">
-        <v>27.66526637591191</v>
+        <v>27.45592096703784</v>
       </c>
       <c r="G478" t="n">
-        <v>24.10471489898362</v>
+        <v>23.74530986258345</v>
       </c>
       <c r="H478" t="n">
-        <v>27.26919983276601</v>
+        <v>27.16227386359932</v>
       </c>
       <c r="I478" t="n">
-        <v>22.03691657102397</v>
+        <v>21.97321317815087</v>
       </c>
       <c r="J478" t="n">
-        <v>20.73086482465914</v>
+        <v>20.5386918910885</v>
       </c>
       <c r="K478" t="n">
-        <v>18.02934128025363</v>
+        <v>17.96929155074893</v>
       </c>
       <c r="L478" t="n">
-        <v>25.37325143890968</v>
+        <v>25.31138640781714</v>
       </c>
       <c r="M478" t="n">
-        <v>21.36026564407395</v>
+        <v>21.11813693770783</v>
       </c>
       <c r="N478" t="n">
-        <v>21.69193348125704</v>
+        <v>21.42596142757312</v>
       </c>
       <c r="O478" t="n">
-        <v>25.14990191475213</v>
+        <v>25.08736859380204</v>
       </c>
       <c r="P478" t="n">
-        <v>24.2840447497944</v>
+        <v>24.17308561200931</v>
       </c>
       <c r="Q478" t="n">
-        <v>20.07013587259373</v>
+        <v>20.145633726654</v>
       </c>
       <c r="R478" t="n">
-        <v>26.35965067359058</v>
+        <v>26.26217210606102</v>
       </c>
       <c r="S478" t="n">
-        <v>20.88590315518978</v>
+        <v>20.93057524461428</v>
       </c>
       <c r="T478" t="n">
-        <v>22.41987172581228</v>
+        <v>22.38658039088384</v>
       </c>
       <c r="U478" t="n">
-        <v>27.53287691873146</v>
+        <v>27.11993377392492</v>
       </c>
       <c r="V478" t="n">
-        <v>28.16157521996682</v>
+        <v>28.16817463414666</v>
       </c>
       <c r="W478" t="n">
-        <v>22.55168941522357</v>
+        <v>22.52208170485568</v>
       </c>
       <c r="X478" t="n">
-        <v>18.27373762124121</v>
+        <v>18.40096076511919</v>
       </c>
       <c r="Y478" t="n">
-        <v>19.85561485093874</v>
+        <v>19.90269198020296</v>
       </c>
       <c r="Z478" t="n">
-        <v>15.32820032749379</v>
+        <v>15.46203534169705</v>
       </c>
       <c r="AA478" t="n">
-        <v>18.53077830369309</v>
+        <v>18.4819493209029</v>
       </c>
       <c r="AB478" t="n">
-        <v>19.07441550875996</v>
+        <v>19.05237010967975</v>
       </c>
       <c r="AC478" t="n">
-        <v>15.94661650863707</v>
+        <v>16.08328273737014</v>
       </c>
       <c r="AD478" t="n">
-        <v>17.05298728518014</v>
+        <v>17.19056210117211</v>
       </c>
       <c r="AE478" t="n">
-        <v>25.28985832732</v>
+        <v>25.3365757174524</v>
       </c>
       <c r="AF478" t="n">
-        <v>23.45401982009267</v>
+        <v>23.10750854863661</v>
       </c>
       <c r="AG478" t="n">
-        <v>22.45679189129502</v>
+        <v>22.40196298233921</v>
       </c>
       <c r="AH478" t="n">
-        <v>26.9992948493856</v>
+        <v>26.86756139932091</v>
       </c>
       <c r="AI478" t="n">
-        <v>21.34481841790359</v>
+        <v>21.38901291214282</v>
       </c>
       <c r="AJ478" t="n">
-        <v>28.63462340840664</v>
+        <v>28.57526263044227</v>
       </c>
       <c r="AK478" t="n">
-        <v>18.72670923055239</v>
+        <v>18.7194937848635</v>
       </c>
       <c r="AL478" t="n">
-        <v>28.42175222099872</v>
+        <v>28.02799058146273</v>
       </c>
       <c r="AM478" t="n">
-        <v>23.59438903263785</v>
+        <v>23.6190654842313</v>
       </c>
     </row>
     <row r="479">
       <c r="A479" s="2" t="n">
-        <v>45199</v>
+        <v>45200</v>
       </c>
       <c r="B479" t="n">
-        <v>21.45392190300358</v>
+        <v>21.3980448263845</v>
       </c>
       <c r="C479" t="n">
-        <v>18.95768910721485</v>
+        <v>18.77676120503044</v>
       </c>
       <c r="D479" t="n">
-        <v>18.75681371363106</v>
+        <v>18.65775837267961</v>
       </c>
       <c r="E479" t="n">
-        <v>22.98964347697253</v>
+        <v>23.03564488429113</v>
       </c>
       <c r="F479" t="n">
-        <v>28.07408412665682</v>
+        <v>28.23793607593377</v>
       </c>
       <c r="G479" t="n">
-        <v>23.57455996226619</v>
+        <v>23.61609241053831</v>
       </c>
       <c r="H479" t="n">
-        <v>27.20363983319244</v>
+        <v>27.49065260051125</v>
       </c>
       <c r="I479" t="n">
-        <v>22.43560596294006</v>
+        <v>22.57731763721636</v>
       </c>
       <c r="J479" t="n">
-        <v>20.75028544195668</v>
+        <v>20.69626388611426</v>
       </c>
       <c r="K479" t="n">
-        <v>18.48770061782297</v>
+        <v>18.36038718974528</v>
       </c>
       <c r="L479" t="n">
-        <v>25.89655034325166</v>
+        <v>26.13884282195319</v>
       </c>
       <c r="M479" t="n">
-        <v>21.51045318355542</v>
+        <v>21.41736858236835</v>
       </c>
       <c r="N479" t="n">
-        <v>21.6361141674451</v>
+        <v>21.59331604445364</v>
       </c>
       <c r="O479" t="n">
-        <v>25.49419897545015</v>
+        <v>25.66794605893429</v>
       </c>
       <c r="P479" t="n">
-        <v>24.74558401575053</v>
+        <v>25.06779930644506</v>
       </c>
       <c r="Q479" t="n">
-        <v>20.50147117653237</v>
+        <v>20.5099389836027</v>
       </c>
       <c r="R479" t="n">
-        <v>27.0162926689701</v>
+        <v>27.12234149313668</v>
       </c>
       <c r="S479" t="n">
-        <v>21.57907407466008</v>
+        <v>21.59714530719915</v>
       </c>
       <c r="T479" t="n">
-        <v>22.88686266290021</v>
+        <v>23.05047998939927</v>
       </c>
       <c r="U479" t="n">
-        <v>26.74226440909406</v>
+        <v>26.9581163666305</v>
       </c>
       <c r="V479" t="n">
-        <v>28.05575490729991</v>
+        <v>28.28768422416486</v>
       </c>
       <c r="W479" t="n">
-        <v>22.57114962534745</v>
+        <v>22.71360587193707</v>
       </c>
       <c r="X479" t="n">
-        <v>19.08004050498344</v>
+        <v>19.04604985599502</v>
       </c>
       <c r="Y479" t="n">
-        <v>20.48193546628259</v>
+        <v>20.49056422665819</v>
       </c>
       <c r="Z479" t="n">
-        <v>16.27676625446013</v>
+        <v>16.11179465450675</v>
       </c>
       <c r="AA479" t="n">
-        <v>18.82120478180965</v>
+        <v>18.73003801280101</v>
       </c>
       <c r="AB479" t="n">
-        <v>19.91750905921291</v>
+        <v>19.78691170354461</v>
       </c>
       <c r="AC479" t="n">
-        <v>16.91973851415388</v>
+        <v>16.70825514380303</v>
       </c>
       <c r="AD479" t="n">
-        <v>17.81320300655605</v>
+        <v>17.74381154989114</v>
       </c>
       <c r="AE479" t="n">
-        <v>25.30829990422564</v>
+        <v>25.49348285886779</v>
       </c>
       <c r="AF479" t="n">
-        <v>22.98899853542438</v>
+        <v>23.02631651050148</v>
       </c>
       <c r="AG479" t="n">
-        <v>22.98900405603906</v>
+        <v>23.33454097314505</v>
       </c>
       <c r="AH479" t="n">
-        <v>27.40744623785444</v>
+        <v>27.5748027587775</v>
       </c>
       <c r="AI479" t="n">
-        <v>21.76559497074816</v>
+        <v>21.82300908457808</v>
       </c>
       <c r="AJ479" t="n">
-        <v>28.57345128157834</v>
+        <v>28.62555156755223</v>
       </c>
       <c r="AK479" t="n">
-        <v>18.96318902627008</v>
+        <v>18.87975120357253</v>
       </c>
       <c r="AL479" t="n">
-        <v>27.92044091545316</v>
+        <v>28.25643798689208</v>
       </c>
       <c r="AM479" t="n">
-        <v>23.94434717176465</v>
+        <v>23.89256484138837</v>
       </c>
     </row>
     <row r="480">
       <c r="A480" s="2" t="n">
-        <v>45230</v>
+        <v>45231</v>
       </c>
       <c r="B480" t="n">
-        <v>20.63454983200797</v>
+        <v>20.62917979775522</v>
       </c>
       <c r="C480" t="n">
-        <v>18.10813929531</v>
+        <v>18.3426186007418</v>
       </c>
       <c r="D480" t="n">
-        <v>18.45167802434985</v>
+        <v>18.4105156260339</v>
       </c>
       <c r="E480" t="n">
-        <v>22.26566656596626</v>
+        <v>22.26305290935187</v>
       </c>
       <c r="F480" t="n">
-        <v>27.80919560201196</v>
+        <v>28.01018452634804</v>
       </c>
       <c r="G480" t="n">
-        <v>22.56449944987313</v>
+        <v>22.77393535378584</v>
       </c>
       <c r="H480" t="n">
-        <v>26.63709926969846</v>
+        <v>26.58350906081021</v>
       </c>
       <c r="I480" t="n">
-        <v>22.0957773135144</v>
+        <v>22.0982411735996</v>
       </c>
       <c r="J480" t="n">
-        <v>20.27493815812748</v>
+        <v>20.37445924294404</v>
       </c>
       <c r="K480" t="n">
-        <v>17.77151035451055</v>
+        <v>17.93030418841774</v>
       </c>
       <c r="L480" t="n">
-        <v>26.40642877294425</v>
+        <v>26.643597620166</v>
       </c>
       <c r="M480" t="n">
-        <v>20.43924153284897</v>
+        <v>20.71045643148546</v>
       </c>
       <c r="N480" t="n">
-        <v>20.78056445975263</v>
+        <v>21.04507043516879</v>
       </c>
       <c r="O480" t="n">
-        <v>25.03781717137009</v>
+        <v>25.11680725885945</v>
       </c>
       <c r="P480" t="n">
-        <v>25.44940310344218</v>
+        <v>25.69703136565594</v>
       </c>
       <c r="Q480" t="n">
-        <v>19.70401217136516</v>
+        <v>19.61271268067826</v>
       </c>
       <c r="R480" t="n">
-        <v>27.37455814759631</v>
+        <v>27.63486322106165</v>
       </c>
       <c r="S480" t="n">
-        <v>21.08266889118629</v>
+        <v>21.02025055999036</v>
       </c>
       <c r="T480" t="n">
-        <v>22.78026157361061</v>
+        <v>22.76907184414599</v>
       </c>
       <c r="U480" t="n">
-        <v>25.93861231632492</v>
+        <v>26.03846854613917</v>
       </c>
       <c r="V480" t="n">
-        <v>27.48528092402707</v>
+        <v>27.49447160025665</v>
       </c>
       <c r="W480" t="n">
-        <v>21.75322276777298</v>
+        <v>21.69830695672297</v>
       </c>
       <c r="X480" t="n">
-        <v>18.56869391314564</v>
+        <v>18.54305250321869</v>
       </c>
       <c r="Y480" t="n">
-        <v>19.89406546696132</v>
+        <v>19.85625916611035</v>
       </c>
       <c r="Z480" t="n">
-        <v>15.81272012042953</v>
+        <v>15.86109401580227</v>
       </c>
       <c r="AA480" t="n">
-        <v>18.28912419062804</v>
+        <v>18.31157896288649</v>
       </c>
       <c r="AB480" t="n">
-        <v>19.20249149473871</v>
+        <v>19.32469410937218</v>
       </c>
       <c r="AC480" t="n">
-        <v>16.27236830000172</v>
+        <v>16.32711830027387</v>
       </c>
       <c r="AD480" t="n">
-        <v>17.27605511969119</v>
+        <v>17.24876935223545</v>
       </c>
       <c r="AE480" t="n">
-        <v>24.50331305981812</v>
+        <v>24.42396958295254</v>
       </c>
       <c r="AF480" t="n">
-        <v>22.44293721933381</v>
+        <v>22.61578703349668</v>
       </c>
       <c r="AG480" t="n">
-        <v>23.52878376413418</v>
+        <v>23.70591404639801</v>
       </c>
       <c r="AH480" t="n">
-        <v>27.08441413617486</v>
+        <v>27.35837051240487</v>
       </c>
       <c r="AI480" t="n">
-        <v>20.93876091911071</v>
+        <v>20.93243543204294</v>
       </c>
       <c r="AJ480" t="n">
-        <v>27.6641654891665</v>
+        <v>27.73385725200134</v>
       </c>
       <c r="AK480" t="n">
-        <v>18.42542018002118</v>
+        <v>18.39688573395022</v>
       </c>
       <c r="AL480" t="n">
-        <v>27.52983202232377</v>
+        <v>27.56562429455866</v>
       </c>
       <c r="AM480" t="n">
-        <v>23.08707755990312</v>
+        <v>23.06389310606659</v>
       </c>
     </row>
     <row r="481">
       <c r="A481" s="2" t="n">
-        <v>45260</v>
+        <v>45261</v>
       </c>
       <c r="B481" t="n">
-        <v>19.93462152197824</v>
+        <v>20.26237517844412</v>
       </c>
       <c r="C481" t="n">
-        <v>18.02438153796248</v>
+        <v>18.39005445512043</v>
       </c>
       <c r="D481" t="n">
-        <v>17.90085966189805</v>
+        <v>18.21203430609622</v>
       </c>
       <c r="E481" t="n">
-        <v>22.0042274157309</v>
+        <v>22.07823229605612</v>
       </c>
       <c r="F481" t="n">
-        <v>28.07985000442829</v>
+        <v>28.32966330947512</v>
       </c>
       <c r="G481" t="n">
-        <v>22.32298487548818</v>
+        <v>22.81050772890798</v>
       </c>
       <c r="H481" t="n">
-        <v>26.05186949624491</v>
+        <v>26.31178160012853</v>
       </c>
       <c r="I481" t="n">
-        <v>21.64223672782228</v>
+        <v>21.75903839005776</v>
       </c>
       <c r="J481" t="n">
-        <v>19.92598026400347</v>
+        <v>20.30793278788697</v>
       </c>
       <c r="K481" t="n">
-        <v>17.48167689664992</v>
+        <v>17.79602895427445</v>
       </c>
       <c r="L481" t="n">
-        <v>27.42122078386717</v>
+        <v>27.23594619477262</v>
       </c>
       <c r="M481" t="n">
-        <v>20.26673285636213</v>
+        <v>20.70667247566258</v>
       </c>
       <c r="N481" t="n">
-        <v>20.64855603569598</v>
+        <v>21.08290213722522</v>
       </c>
       <c r="O481" t="n">
-        <v>25.19818671999921</v>
+        <v>25.28244794690746</v>
       </c>
       <c r="P481" t="n">
-        <v>26.56316726694317</v>
+        <v>26.36441473239053</v>
       </c>
       <c r="Q481" t="n">
-        <v>18.73172578070333</v>
+        <v>18.92920123526882</v>
       </c>
       <c r="R481" t="n">
-        <v>28.04021768121159</v>
+        <v>28.06705853526937</v>
       </c>
       <c r="S481" t="n">
-        <v>20.46854632606042</v>
+        <v>20.60167797245605</v>
       </c>
       <c r="T481" t="n">
-        <v>22.5408550710274</v>
+        <v>22.55224685549195</v>
       </c>
       <c r="U481" t="n">
-        <v>25.20585121321858</v>
+        <v>25.73820431331492</v>
       </c>
       <c r="V481" t="n">
-        <v>26.92014273614914</v>
+        <v>27.41997401708553</v>
       </c>
       <c r="W481" t="n">
-        <v>21.1169845258612</v>
+        <v>21.25749073391539</v>
       </c>
       <c r="X481" t="n">
-        <v>18.12292962158419</v>
+        <v>18.22551003927135</v>
       </c>
       <c r="Y481" t="n">
-        <v>19.31880197116239</v>
+        <v>19.48421490111715</v>
       </c>
       <c r="Z481" t="n">
-        <v>15.45314238884272</v>
+        <v>15.7062164824659</v>
       </c>
       <c r="AA481" t="n">
-        <v>17.74523673143588</v>
+        <v>18.05790688867426</v>
       </c>
       <c r="AB481" t="n">
-        <v>18.83717273523219</v>
+        <v>19.22639822007681</v>
       </c>
       <c r="AC481" t="n">
-        <v>15.83222374787525</v>
+        <v>16.08499131755057</v>
       </c>
       <c r="AD481" t="n">
-        <v>16.73874635550775</v>
+        <v>16.84621837147573</v>
       </c>
       <c r="AE481" t="n">
-        <v>23.69940382750619</v>
+        <v>23.94131639242378</v>
       </c>
       <c r="AF481" t="n">
-        <v>22.25998644284504</v>
+        <v>22.76376207144744</v>
       </c>
       <c r="AG481" t="n">
-        <v>24.15467545243181</v>
+        <v>23.94441715863345</v>
       </c>
       <c r="AH481" t="n">
-        <v>27.85740786696505</v>
+        <v>27.98485823952867</v>
       </c>
       <c r="AI481" t="n">
-        <v>20.57767009719546</v>
+        <v>20.64670790649133</v>
       </c>
       <c r="AJ481" t="n">
-        <v>26.86230763317481</v>
+        <v>27.50428747066106</v>
       </c>
       <c r="AK481" t="n">
-        <v>17.81218171493562</v>
+        <v>18.12843251905397</v>
       </c>
       <c r="AL481" t="n">
-        <v>26.95440619516141</v>
+        <v>27.44306557982275</v>
       </c>
       <c r="AM481" t="n">
-        <v>22.34659996343616</v>
+        <v>22.80866417659915</v>
       </c>
     </row>
     <row r="482">
       <c r="A482" s="2" t="n">
-        <v>45291</v>
+        <v>45292</v>
       </c>
       <c r="B482" t="n">
-        <v>21.26261859847078</v>
+        <v>21.02370383230943</v>
       </c>
       <c r="C482" t="n">
-        <v>19.45576459339421</v>
+        <v>19.02961624720447</v>
       </c>
       <c r="D482" t="n">
-        <v>19.00486809557108</v>
+        <v>18.94099511874499</v>
       </c>
       <c r="E482" t="n">
-        <v>22.92943919195035</v>
+        <v>22.80158060748323</v>
       </c>
       <c r="F482" t="n">
-        <v>29.68130103068765</v>
+        <v>29.3220070311431</v>
       </c>
       <c r="G482" t="n">
-        <v>23.77673430943452</v>
+        <v>23.39420103483327</v>
       </c>
       <c r="H482" t="n">
-        <v>27.60506350042613</v>
+        <v>27.16905693049616</v>
       </c>
       <c r="I482" t="n">
-        <v>22.30281630259362</v>
+        <v>22.23789307265483</v>
       </c>
       <c r="J482" t="n">
-        <v>21.32244228454839</v>
+        <v>21.06369999483028</v>
       </c>
       <c r="K482" t="n">
-        <v>18.71420820086979</v>
+        <v>18.37868212718111</v>
       </c>
       <c r="L482" t="n">
-        <v>27.96437569312523</v>
+        <v>27.80736717512738</v>
       </c>
       <c r="M482" t="n">
-        <v>21.73087060958084</v>
+        <v>21.28890446382055</v>
       </c>
       <c r="N482" t="n">
-        <v>22.24951407879543</v>
+        <v>21.81310561307415</v>
       </c>
       <c r="O482" t="n">
-        <v>26.49678439886877</v>
+        <v>26.27566028374887</v>
       </c>
       <c r="P482" t="n">
-        <v>27.2706110572441</v>
+        <v>27.09940931918934</v>
       </c>
       <c r="Q482" t="n">
-        <v>19.65480339128444</v>
+        <v>19.46022382534026</v>
       </c>
       <c r="R482" t="n">
-        <v>28.52178593411815</v>
+        <v>28.25555895065756</v>
       </c>
       <c r="S482" t="n">
-        <v>21.26101906223601</v>
+        <v>21.17451078457659</v>
       </c>
       <c r="T482" t="n">
-        <v>23.21737726272072</v>
+        <v>23.13909972055929</v>
       </c>
       <c r="U482" t="n">
-        <v>27.56202985418486</v>
+        <v>26.99739144683765</v>
       </c>
       <c r="V482" t="n">
-        <v>29.39844923738843</v>
+        <v>28.63910614172899</v>
       </c>
       <c r="W482" t="n">
-        <v>22.18293029621003</v>
+        <v>21.92404402119203</v>
       </c>
       <c r="X482" t="n">
-        <v>18.95201688815792</v>
+        <v>18.79708902192122</v>
       </c>
       <c r="Y482" t="n">
-        <v>20.21096106414651</v>
+        <v>20.09477297162684</v>
       </c>
       <c r="Z482" t="n">
-        <v>16.51911318839025</v>
+        <v>16.25992295218731</v>
       </c>
       <c r="AA482" t="n">
-        <v>18.94680304234477</v>
+        <v>18.72904175670947</v>
       </c>
       <c r="AB482" t="n">
-        <v>20.16398629380609</v>
+        <v>19.84249976937175</v>
       </c>
       <c r="AC482" t="n">
-        <v>16.91128658167133</v>
+        <v>16.64268434837368</v>
       </c>
       <c r="AD482" t="n">
-        <v>17.51666025407892</v>
+        <v>17.35301610203893</v>
       </c>
       <c r="AE482" t="n">
-        <v>24.96767507392794</v>
+        <v>24.62390706535145</v>
       </c>
       <c r="AF482" t="n">
-        <v>23.9433785445413</v>
+        <v>23.56207502045784</v>
       </c>
       <c r="AG482" t="n">
-        <v>24.82745169429983</v>
+        <v>24.69233386470349</v>
       </c>
       <c r="AH482" t="n">
-        <v>29.48465021025677</v>
+        <v>29.12946964389527</v>
       </c>
       <c r="AI482" t="n">
-        <v>21.45655915652426</v>
+        <v>21.28870971892704</v>
       </c>
       <c r="AJ482" t="n">
-        <v>29.24314221175091</v>
+        <v>28.57249020381486</v>
       </c>
       <c r="AK482" t="n">
-        <v>19.07221986092345</v>
+        <v>18.92255982076964</v>
       </c>
       <c r="AL482" t="n">
-        <v>29.25742246000478</v>
+        <v>28.76430561673558</v>
       </c>
       <c r="AM482" t="n">
-        <v>24.13541399118088</v>
+        <v>23.8107882030292</v>
       </c>
     </row>
     <row r="483">
       <c r="A483" s="2" t="n">
-        <v>45322</v>
+        <v>45323</v>
       </c>
       <c r="B483" t="n">
-        <v>22.65989307549331</v>
+        <v>22.24222984369296</v>
       </c>
       <c r="C483" t="n">
-        <v>20.47483034443212</v>
+        <v>19.9168880367342</v>
       </c>
       <c r="D483" t="n">
-        <v>20.47215924749366</v>
+        <v>20.23634685625091</v>
       </c>
       <c r="E483" t="n">
-        <v>24.32180613928886</v>
+        <v>24.01915500008804</v>
       </c>
       <c r="F483" t="n">
-        <v>30.44593034184189</v>
+        <v>30.23691831577407</v>
       </c>
       <c r="G483" t="n">
-        <v>24.9131436773484</v>
+        <v>24.27459244291423</v>
       </c>
       <c r="H483" t="n">
-        <v>28.66748666400902</v>
+        <v>28.40215698569172</v>
       </c>
       <c r="I483" t="n">
-        <v>23.82856082157004</v>
+        <v>23.31594401049235</v>
       </c>
       <c r="J483" t="n">
-        <v>22.49436432896209</v>
+        <v>22.15468089133174</v>
       </c>
       <c r="K483" t="n">
-        <v>19.76176963276544</v>
+        <v>19.3463182627682</v>
       </c>
       <c r="L483" t="n">
-        <v>28.41450203033982</v>
+        <v>28.32940774675146</v>
       </c>
       <c r="M483" t="n">
-        <v>22.81023320446677</v>
+        <v>22.19649661961726</v>
       </c>
       <c r="N483" t="n">
-        <v>23.34094645183602</v>
+        <v>22.78304282491588</v>
       </c>
       <c r="O483" t="n">
-        <v>27.64707832075087</v>
+        <v>27.36931045469176</v>
       </c>
       <c r="P483" t="n">
-        <v>27.72835232551165</v>
+        <v>27.63750225219912</v>
       </c>
       <c r="Q483" t="n">
-        <v>20.96572256803161</v>
+        <v>20.64214511511775</v>
       </c>
       <c r="R483" t="n">
-        <v>28.7229612533472</v>
+        <v>28.59578416913237</v>
       </c>
       <c r="S483" t="n">
-        <v>22.83423522814801</v>
+        <v>22.40795929075678</v>
       </c>
       <c r="T483" t="n">
-        <v>24.62196609227048</v>
+        <v>24.24729199639511</v>
       </c>
       <c r="U483" t="n">
-        <v>28.60167260705989</v>
+        <v>28.3762139564723</v>
       </c>
       <c r="V483" t="n">
-        <v>30.44300875001461</v>
+        <v>29.83761722928016</v>
       </c>
       <c r="W483" t="n">
-        <v>23.31301716308711</v>
+        <v>23.07274866974991</v>
       </c>
       <c r="X483" t="n">
-        <v>20.25686430241977</v>
+        <v>19.91158588239851</v>
       </c>
       <c r="Y483" t="n">
-        <v>21.75355470717093</v>
+        <v>21.27630482653696</v>
       </c>
       <c r="Z483" t="n">
-        <v>17.64128602932531</v>
+        <v>17.21183131698749</v>
       </c>
       <c r="AA483" t="n">
-        <v>20.22934500386445</v>
+        <v>19.88536447665721</v>
       </c>
       <c r="AB483" t="n">
-        <v>21.3831052817141</v>
+        <v>20.74345322027806</v>
       </c>
       <c r="AC483" t="n">
-        <v>17.96136751476264</v>
+        <v>17.61135330838107</v>
       </c>
       <c r="AD483" t="n">
-        <v>18.72739004558533</v>
+        <v>18.43691303718235</v>
       </c>
       <c r="AE483" t="n">
-        <v>26.15055970259325</v>
+        <v>25.79999818524769</v>
       </c>
       <c r="AF483" t="n">
-        <v>24.93863597150754</v>
+        <v>24.4640108014008</v>
       </c>
       <c r="AG483" t="n">
-        <v>25.74182962604323</v>
+        <v>25.51232367500564</v>
       </c>
       <c r="AH483" t="n">
-        <v>30.25277540927264</v>
+        <v>30.04556738817146</v>
       </c>
       <c r="AI483" t="n">
-        <v>22.72007250796114</v>
+        <v>22.46769016873785</v>
       </c>
       <c r="AJ483" t="n">
-        <v>30.3991819429582</v>
+        <v>29.80502908234547</v>
       </c>
       <c r="AK483" t="n">
-        <v>20.67299826595118</v>
+        <v>20.30173817508584</v>
       </c>
       <c r="AL483" t="n">
-        <v>30.53633066881697</v>
+        <v>30.13377165922308</v>
       </c>
       <c r="AM483" t="n">
-        <v>25.50852591456545</v>
+        <v>25.10041060921816</v>
       </c>
     </row>
     <row r="484">
       <c r="A484" s="2" t="n">
-        <v>45351</v>
+        <v>45352</v>
       </c>
       <c r="B484" t="n">
-        <v>22.32003217994582</v>
+        <v>22.9168908312234</v>
       </c>
       <c r="C484" t="n">
-        <v>19.3753875014827</v>
+        <v>20.32417967162711</v>
       </c>
       <c r="D484" t="n">
-        <v>20.54845933852892</v>
+        <v>20.93974880070609</v>
       </c>
       <c r="E484" t="n">
-        <v>23.89282210205072</v>
+        <v>24.47964754025279</v>
       </c>
       <c r="F484" t="n">
-        <v>30.28291199565968</v>
+        <v>30.58046531652599</v>
       </c>
       <c r="G484" t="n">
-        <v>23.63082708719442</v>
+        <v>24.33490805755985</v>
       </c>
       <c r="H484" t="n">
-        <v>28.54916565335445</v>
+        <v>29.12987387841847</v>
       </c>
       <c r="I484" t="n">
-        <v>22.76538588199642</v>
+        <v>23.49165193569332</v>
       </c>
       <c r="J484" t="n">
-        <v>22.14622842054962</v>
+        <v>22.69120019722605</v>
       </c>
       <c r="K484" t="n">
-        <v>19.26475142828382</v>
+        <v>20.00305834496776</v>
       </c>
       <c r="L484" t="n">
-        <v>28.17101910495036</v>
+        <v>28.49478520524983</v>
       </c>
       <c r="M484" t="n">
-        <v>21.59826604034161</v>
+        <v>22.49210373692905</v>
       </c>
       <c r="N484" t="n">
-        <v>22.35475364849252</v>
+        <v>23.15400516009244</v>
       </c>
       <c r="O484" t="n">
-        <v>26.99833546012886</v>
+        <v>27.57437914041475</v>
       </c>
       <c r="P484" t="n">
-        <v>27.1378781642208</v>
+        <v>27.47619405735141</v>
       </c>
       <c r="Q484" t="n">
-        <v>20.82398056882314</v>
+        <v>21.36538359825363</v>
       </c>
       <c r="R484" t="n">
-        <v>28.96288215792815</v>
+        <v>29.20003982721731</v>
       </c>
       <c r="S484" t="n">
-        <v>22.13668809842112</v>
+        <v>22.83781917413103</v>
       </c>
       <c r="T484" t="n">
-        <v>23.85661615106054</v>
+        <v>24.56277840971717</v>
       </c>
       <c r="U484" t="n">
-        <v>28.88413711074997</v>
+        <v>29.2337980065407</v>
       </c>
       <c r="V484" t="n">
-        <v>29.1315780542098</v>
+        <v>30.17606945031251</v>
       </c>
       <c r="W484" t="n">
-        <v>23.25405228160692</v>
+        <v>23.77355959269459</v>
       </c>
       <c r="X484" t="n">
-        <v>19.69790644956362</v>
+        <v>20.35324839125701</v>
       </c>
       <c r="Y484" t="n">
-        <v>20.86233905346473</v>
+        <v>21.58327490388909</v>
       </c>
       <c r="Z484" t="n">
-        <v>16.99627979759084</v>
+        <v>17.77048728829203</v>
       </c>
       <c r="AA484" t="n">
-        <v>20.04401540326347</v>
+        <v>20.65470854788967</v>
       </c>
       <c r="AB484" t="n">
-        <v>19.95686502771981</v>
+        <v>20.92855790946002</v>
       </c>
       <c r="AC484" t="n">
-        <v>17.5711758828369</v>
+        <v>18.29323709987012</v>
       </c>
       <c r="AD484" t="n">
-        <v>18.42565852072572</v>
+        <v>18.98375893417452</v>
       </c>
       <c r="AE484" t="n">
-        <v>25.92918078144969</v>
+        <v>26.47456883389704</v>
       </c>
       <c r="AF484" t="n">
-        <v>24.03615830530425</v>
+        <v>24.61562809928304</v>
       </c>
       <c r="AG484" t="n">
-        <v>24.92674885896737</v>
+        <v>25.46697604045855</v>
       </c>
       <c r="AH484" t="n">
-        <v>29.6700083191868</v>
+        <v>30.04898930865477</v>
       </c>
       <c r="AI484" t="n">
-        <v>22.52423876582434</v>
+        <v>23.05607929941388</v>
       </c>
       <c r="AJ484" t="n">
-        <v>29.35190072289696</v>
+        <v>30.18923952100007</v>
       </c>
       <c r="AK484" t="n">
-        <v>20.49306144420867</v>
+        <v>21.06932920400171</v>
       </c>
       <c r="AL484" t="n">
-        <v>30.03857221215144</v>
+        <v>30.60379137402202</v>
       </c>
       <c r="AM484" t="n">
-        <v>25.08447553064633</v>
+        <v>25.63365493159433</v>
       </c>
     </row>
     <row r="485">
       <c r="A485" s="2" t="n">
-        <v>45382</v>
+        <v>45383</v>
       </c>
       <c r="B485" t="n">
-        <v>22.14995147552535</v>
+        <v>21.99423864823527</v>
       </c>
       <c r="C485" t="n">
-        <v>19.00229880976869</v>
+        <v>18.59886982132483</v>
       </c>
       <c r="D485" t="n">
-        <v>20.10515999918627</v>
+        <v>19.7334501802014</v>
       </c>
       <c r="E485" t="n">
-        <v>23.57220659357599</v>
+        <v>23.30070083249367</v>
       </c>
       <c r="F485" t="n">
-        <v>29.18418645766575</v>
+        <v>28.92549234280187</v>
       </c>
       <c r="G485" t="n">
-        <v>23.16306240130645</v>
+        <v>22.88111931358664</v>
       </c>
       <c r="H485" t="n">
-        <v>27.93785995066682</v>
+        <v>27.78573559369636</v>
       </c>
       <c r="I485" t="n">
-        <v>22.41429998808194</v>
+        <v>21.99863852554469</v>
       </c>
       <c r="J485" t="n">
-        <v>21.63554523480438</v>
+        <v>21.24258261632912</v>
       </c>
       <c r="K485" t="n">
-        <v>19.02063399834206</v>
+        <v>18.67713413595201</v>
       </c>
       <c r="L485" t="n">
-        <v>27.48977961418808</v>
+        <v>27.23113382908662</v>
       </c>
       <c r="M485" t="n">
-        <v>21.19807391007131</v>
+        <v>20.79956239726405</v>
       </c>
       <c r="N485" t="n">
-        <v>21.87848128386069</v>
+        <v>21.52281607161704</v>
       </c>
       <c r="O485" t="n">
-        <v>26.40718245465246</v>
+        <v>26.01326942577609</v>
       </c>
       <c r="P485" t="n">
-        <v>26.12403678573325</v>
+        <v>25.83089521411081</v>
       </c>
       <c r="Q485" t="n">
-        <v>20.82468517254064</v>
+        <v>20.83197645754496</v>
       </c>
       <c r="R485" t="n">
-        <v>28.73427016647284</v>
+        <v>28.66595069991628</v>
       </c>
       <c r="S485" t="n">
-        <v>21.86571881785133</v>
+        <v>21.60127032753892</v>
       </c>
       <c r="T485" t="n">
-        <v>23.55573880880114</v>
+        <v>23.18009551182898</v>
       </c>
       <c r="U485" t="n">
-        <v>27.42325548132501</v>
+        <v>27.31289398053546</v>
       </c>
       <c r="V485" t="n">
-        <v>28.29502285185656</v>
+        <v>28.2223783832938</v>
       </c>
       <c r="W485" t="n">
-        <v>23.03219323162192</v>
+        <v>22.92749909843145</v>
       </c>
       <c r="X485" t="n">
-        <v>19.46945407615638</v>
+        <v>19.285840595297</v>
       </c>
       <c r="Y485" t="n">
-        <v>20.52130388540116</v>
+        <v>20.26461106323044</v>
       </c>
       <c r="Z485" t="n">
-        <v>16.88637956671185</v>
+        <v>16.5958871962011</v>
       </c>
       <c r="AA485" t="n">
-        <v>19.81780822855037</v>
+        <v>19.50442781858153</v>
       </c>
       <c r="AB485" t="n">
-        <v>19.57161712429359</v>
+        <v>19.13057664738213</v>
       </c>
       <c r="AC485" t="n">
-        <v>17.5518102791108</v>
+        <v>17.25712719657628</v>
       </c>
       <c r="AD485" t="n">
-        <v>18.2497360797165</v>
+        <v>18.19542675563074</v>
       </c>
       <c r="AE485" t="n">
-        <v>25.70131113781619</v>
+        <v>25.74470152294607</v>
       </c>
       <c r="AF485" t="n">
-        <v>23.37251068247022</v>
+        <v>23.00712065767953</v>
       </c>
       <c r="AG485" t="n">
-        <v>24.11967131502106</v>
+        <v>23.74557710334325</v>
       </c>
       <c r="AH485" t="n">
-        <v>28.47688452522108</v>
+        <v>28.14910814604561</v>
       </c>
       <c r="AI485" t="n">
-        <v>22.27692458712175</v>
+        <v>22.09571014384065</v>
       </c>
       <c r="AJ485" t="n">
-        <v>28.70641150912202</v>
+        <v>28.65536247033942</v>
       </c>
       <c r="AK485" t="n">
-        <v>20.21059137638382</v>
+        <v>19.93319910130572</v>
       </c>
       <c r="AL485" t="n">
-        <v>28.69914429436192</v>
+        <v>28.46769247898668</v>
       </c>
       <c r="AM485" t="n">
-        <v>24.61518597472916</v>
+        <v>24.51625781479009</v>
       </c>
     </row>
     <row r="486">
       <c r="A486" s="2" t="n">
-        <v>45412</v>
+        <v>45413</v>
       </c>
       <c r="B486" t="n">
-        <v>21.25012078243515</v>
+        <v>21.17825169386905</v>
       </c>
       <c r="C486" t="n">
-        <v>17.71545658518826</v>
+        <v>17.6857863606534</v>
       </c>
       <c r="D486" t="n">
-        <v>18.80949367839967</v>
+        <v>18.81081215647059</v>
       </c>
       <c r="E486" t="n">
-        <v>22.36825980450022</v>
+        <v>22.3983930794906</v>
       </c>
       <c r="F486" t="n">
-        <v>27.10727526030405</v>
+        <v>27.38392146229015</v>
       </c>
       <c r="G486" t="n">
-        <v>22.27514003964853</v>
+        <v>22.32975711159553</v>
       </c>
       <c r="H486" t="n">
-        <v>27.00478370698181</v>
+        <v>27.01019611814104</v>
       </c>
       <c r="I486" t="n">
-        <v>20.83409568322255</v>
+        <v>20.90518962371278</v>
       </c>
       <c r="J486" t="n">
-        <v>20.43031367376405</v>
+        <v>20.42282679757238</v>
       </c>
       <c r="K486" t="n">
-        <v>17.95298026859344</v>
+        <v>17.92612136263261</v>
       </c>
       <c r="L486" t="n">
-        <v>25.87092145430072</v>
+        <v>25.97285358472321</v>
       </c>
       <c r="M486" t="n">
-        <v>20.0569980571154</v>
+        <v>20.03827386717769</v>
       </c>
       <c r="N486" t="n">
-        <v>20.85496438632481</v>
+        <v>20.8099880756764</v>
       </c>
       <c r="O486" t="n">
-        <v>24.98973439365007</v>
+        <v>25.16126273834463</v>
       </c>
       <c r="P486" t="n">
-        <v>24.45758709450416</v>
+        <v>24.5282420476961</v>
       </c>
       <c r="Q486" t="n">
-        <v>20.37084614102776</v>
+        <v>20.19048899098554</v>
       </c>
       <c r="R486" t="n">
-        <v>27.24270854758449</v>
+        <v>27.34260257707662</v>
       </c>
       <c r="S486" t="n">
-        <v>20.45984750337008</v>
+        <v>20.39032290009851</v>
       </c>
       <c r="T486" t="n">
-        <v>22.07041957378778</v>
+        <v>22.07921964332844</v>
       </c>
       <c r="U486" t="n">
-        <v>26.10982827745354</v>
+        <v>26.0773176797072</v>
       </c>
       <c r="V486" t="n">
-        <v>27.67162845415497</v>
+        <v>27.50256590191894</v>
       </c>
       <c r="W486" t="n">
-        <v>22.3425067904579</v>
+        <v>22.29526140444351</v>
       </c>
       <c r="X486" t="n">
-        <v>18.25241472525652</v>
+        <v>18.18688416681996</v>
       </c>
       <c r="Y486" t="n">
-        <v>19.09656238276949</v>
+        <v>19.05461614018314</v>
       </c>
       <c r="Z486" t="n">
-        <v>15.66671827435905</v>
+        <v>15.67332304596754</v>
       </c>
       <c r="AA486" t="n">
-        <v>18.71223291905807</v>
+        <v>18.66390706688299</v>
       </c>
       <c r="AB486" t="n">
-        <v>18.06676834353684</v>
+        <v>18.03440067383663</v>
       </c>
       <c r="AC486" t="n">
-        <v>16.42431743906157</v>
+        <v>16.42167949768053</v>
       </c>
       <c r="AD486" t="n">
-        <v>17.40562350231393</v>
+        <v>17.28940714468787</v>
       </c>
       <c r="AE486" t="n">
-        <v>25.38572784989943</v>
+        <v>25.29800101510308</v>
       </c>
       <c r="AF486" t="n">
-        <v>22.32345200753899</v>
+        <v>22.39815708292622</v>
       </c>
       <c r="AG486" t="n">
-        <v>22.336786518787</v>
+        <v>22.48474101235726</v>
       </c>
       <c r="AH486" t="n">
-        <v>26.61101377139922</v>
+        <v>26.88726476868879</v>
       </c>
       <c r="AI486" t="n">
-        <v>21.34526895792157</v>
+        <v>21.34364873039963</v>
       </c>
       <c r="AJ486" t="n">
-        <v>28.17594739802843</v>
+        <v>27.96668342240434</v>
       </c>
       <c r="AK486" t="n">
-        <v>19.03460043372144</v>
+        <v>18.98943189819371</v>
       </c>
       <c r="AL486" t="n">
-        <v>27.12724711411975</v>
+        <v>27.1508789477673</v>
       </c>
       <c r="AM486" t="n">
-        <v>23.7395911377437</v>
+        <v>23.57531752535548</v>
       </c>
     </row>
     <row r="487">
       <c r="A487" s="2" t="n">
-        <v>45443</v>
+        <v>45444</v>
       </c>
       <c r="B487" t="n">
-        <v>20.4358800880247</v>
+        <v>20.42851900254546</v>
       </c>
       <c r="C487" t="n">
-        <v>16.91869954435636</v>
+        <v>16.83028439542111</v>
       </c>
       <c r="D487" t="n">
-        <v>17.8627282377121</v>
+        <v>18.02634026874222</v>
       </c>
       <c r="E487" t="n">
-        <v>21.47558749571817</v>
+        <v>21.33862237115338</v>
       </c>
       <c r="F487" t="n">
-        <v>26.26278404880137</v>
+        <v>26.1816117406118</v>
       </c>
       <c r="G487" t="n">
-        <v>21.89381359500961</v>
+        <v>22.04451995584247</v>
       </c>
       <c r="H487" t="n">
-        <v>26.19174741936232</v>
+        <v>26.129016583162</v>
       </c>
       <c r="I487" t="n">
-        <v>20.07122818857854</v>
+        <v>20.09580397507855</v>
       </c>
       <c r="J487" t="n">
-        <v>19.51302335186067</v>
+        <v>19.73081532129785</v>
       </c>
       <c r="K487" t="n">
-        <v>17.12819211166316</v>
+        <v>17.13107995632786</v>
       </c>
       <c r="L487" t="n">
-        <v>24.74448296738704</v>
+        <v>24.75597628199194</v>
       </c>
       <c r="M487" t="n">
-        <v>19.38929924522226</v>
+        <v>19.46804787760806</v>
       </c>
       <c r="N487" t="n">
-        <v>20.04911678844606</v>
+        <v>20.23833471353721</v>
       </c>
       <c r="O487" t="n">
-        <v>24.2228834414451</v>
+        <v>24.15347507872402</v>
       </c>
       <c r="P487" t="n">
-        <v>23.20415817135284</v>
+        <v>23.29132915880581</v>
       </c>
       <c r="Q487" t="n">
-        <v>19.6602364388202</v>
+        <v>19.50440806723885</v>
       </c>
       <c r="R487" t="n">
-        <v>26.17131720542053</v>
+        <v>26.03658793633424</v>
       </c>
       <c r="S487" t="n">
-        <v>19.62061969543475</v>
+        <v>19.50129697236358</v>
       </c>
       <c r="T487" t="n">
-        <v>21.18941145083271</v>
+        <v>21.10165976053309</v>
       </c>
       <c r="U487" t="n">
-        <v>25.48041023883129</v>
+        <v>25.61719471960312</v>
       </c>
       <c r="V487" t="n">
-        <v>26.95508738550351</v>
+        <v>26.85040961513694</v>
       </c>
       <c r="W487" t="n">
-        <v>21.67481246743134</v>
+        <v>21.5613155791294</v>
       </c>
       <c r="X487" t="n">
-        <v>17.45777276444894</v>
+        <v>17.22085220510612</v>
       </c>
       <c r="Y487" t="n">
-        <v>18.41419456367899</v>
+        <v>18.3133692963162</v>
       </c>
       <c r="Z487" t="n">
-        <v>14.94731801784105</v>
+        <v>14.70288455598719</v>
       </c>
       <c r="AA487" t="n">
-        <v>17.81551171859216</v>
+        <v>17.84935517040371</v>
       </c>
       <c r="AB487" t="n">
-        <v>17.28022465223026</v>
+        <v>17.22178625789854</v>
       </c>
       <c r="AC487" t="n">
-        <v>15.7723040477747</v>
+        <v>15.5218162680854</v>
       </c>
       <c r="AD487" t="n">
-        <v>16.66049612548505</v>
+        <v>16.37783515562429</v>
       </c>
       <c r="AE487" t="n">
-        <v>24.60250783412601</v>
+        <v>24.48824806298146</v>
       </c>
       <c r="AF487" t="n">
-        <v>21.73775080142952</v>
+        <v>21.98438697433573</v>
       </c>
       <c r="AG487" t="n">
-        <v>21.25146022428705</v>
+        <v>21.19237720354894</v>
       </c>
       <c r="AH487" t="n">
-        <v>25.87141441679588</v>
+        <v>25.841989032329</v>
       </c>
       <c r="AI487" t="n">
-        <v>20.59549388872138</v>
+        <v>20.44729160130498</v>
       </c>
       <c r="AJ487" t="n">
-        <v>27.34282271029965</v>
+        <v>27.39409674926222</v>
       </c>
       <c r="AK487" t="n">
-        <v>18.17686285773005</v>
+        <v>18.20764359224287</v>
       </c>
       <c r="AL487" t="n">
-        <v>26.30798267882912</v>
+        <v>26.3957539676993</v>
       </c>
       <c r="AM487" t="n">
-        <v>22.69800658914687</v>
+        <v>22.7995672572631</v>
       </c>
     </row>
     <row r="488">
       <c r="A488" s="2" t="n">
-        <v>45473</v>
+        <v>45474</v>
       </c>
       <c r="B488" t="n">
-        <v>19.73335884075244</v>
+        <v>19.64892451348188</v>
       </c>
       <c r="C488" t="n">
-        <v>16.5069284927608</v>
+        <v>16.50582329527602</v>
       </c>
       <c r="D488" t="n">
-        <v>17.51229773521911</v>
+        <v>17.39642388165646</v>
       </c>
       <c r="E488" t="n">
-        <v>20.82304198657361</v>
+        <v>20.76390419094233</v>
       </c>
       <c r="F488" t="n">
-        <v>25.77635876915347</v>
+        <v>25.65945103868575</v>
       </c>
       <c r="G488" t="n">
-        <v>22.2171263485151</v>
+        <v>22.08775086395256</v>
       </c>
       <c r="H488" t="n">
-        <v>25.65762866595473</v>
+        <v>25.52104028368757</v>
       </c>
       <c r="I488" t="n">
-        <v>19.93533678777941</v>
+        <v>19.81682065542451</v>
       </c>
       <c r="J488" t="n">
-        <v>19.34075901398852</v>
+        <v>19.19576567446915</v>
       </c>
       <c r="K488" t="n">
-        <v>16.71871480637722</v>
+        <v>16.6454896212716</v>
       </c>
       <c r="L488" t="n">
-        <v>24.33813577575611</v>
+        <v>24.18673870274493</v>
       </c>
       <c r="M488" t="n">
-        <v>19.4291284560364</v>
+        <v>19.37449199331167</v>
       </c>
       <c r="N488" t="n">
-        <v>20.04204869939151</v>
+        <v>19.89967548614812</v>
       </c>
       <c r="O488" t="n">
-        <v>23.61733012422269</v>
+        <v>23.50533803402202</v>
       </c>
       <c r="P488" t="n">
-        <v>22.89318824307534</v>
+        <v>22.73914594366668</v>
       </c>
       <c r="Q488" t="n">
-        <v>18.88489287439899</v>
+        <v>18.8985648155093</v>
       </c>
       <c r="R488" t="n">
-        <v>25.4471779779963</v>
+        <v>25.39463504192016</v>
       </c>
       <c r="S488" t="n">
-        <v>19.26128952511026</v>
+        <v>19.21321891133719</v>
       </c>
       <c r="T488" t="n">
-        <v>20.79396112353428</v>
+        <v>20.75419349035455</v>
       </c>
       <c r="U488" t="n">
-        <v>25.17448023243625</v>
+        <v>25.12756045207697</v>
       </c>
       <c r="V488" t="n">
-        <v>26.56733929984471</v>
+        <v>26.43955059202611</v>
       </c>
       <c r="W488" t="n">
-        <v>21.11642512308281</v>
+        <v>21.028716057223</v>
       </c>
       <c r="X488" t="n">
-        <v>16.83924803319696</v>
+        <v>16.83728650252048</v>
       </c>
       <c r="Y488" t="n">
-        <v>18.17796059973373</v>
+        <v>18.08141836223133</v>
       </c>
       <c r="Z488" t="n">
-        <v>14.17448744422153</v>
+        <v>14.17035501451495</v>
       </c>
       <c r="AA488" t="n">
-        <v>17.35201994190222</v>
+        <v>17.26952780862309</v>
       </c>
       <c r="AB488" t="n">
-        <v>16.99369916953941</v>
+        <v>17.00686559135701</v>
       </c>
       <c r="AC488" t="n">
-        <v>14.89284949512516</v>
+        <v>14.93304830605416</v>
       </c>
       <c r="AD488" t="n">
-        <v>15.87553922524437</v>
+        <v>15.91358718712184</v>
       </c>
       <c r="AE488" t="n">
-        <v>24.00874211878824</v>
+        <v>23.92874625883919</v>
       </c>
       <c r="AF488" t="n">
-        <v>21.88054898707601</v>
+        <v>21.7053533757142</v>
       </c>
       <c r="AG488" t="n">
-        <v>20.77611618610084</v>
+        <v>20.65790732344686</v>
       </c>
       <c r="AH488" t="n">
-        <v>25.43795230636039</v>
+        <v>25.27815007033537</v>
       </c>
       <c r="AI488" t="n">
-        <v>19.94720884488132</v>
+        <v>19.88264949450637</v>
       </c>
       <c r="AJ488" t="n">
-        <v>26.84875882030424</v>
+        <v>26.82725507453627</v>
       </c>
       <c r="AK488" t="n">
-        <v>17.67383142704983</v>
+        <v>17.58289420590928</v>
       </c>
       <c r="AL488" t="n">
-        <v>26.01023233619754</v>
+        <v>25.93163939607416</v>
       </c>
       <c r="AM488" t="n">
-        <v>22.1494128283505</v>
+        <v>22.06044925911361</v>
       </c>
     </row>
     <row r="489">
       <c r="A489" s="2" t="n">
-        <v>45504</v>
+        <v>45505</v>
       </c>
       <c r="B489" t="n">
-        <v>19.89539129278691</v>
+        <v>19.91558040889785</v>
       </c>
       <c r="C489" t="n">
-        <v>17.05837919333176</v>
+        <v>17.19280734287113</v>
       </c>
       <c r="D489" t="n">
-        <v>17.72450885071505</v>
+        <v>17.86134101788915</v>
       </c>
       <c r="E489" t="n">
-        <v>21.1520164504061</v>
+        <v>21.22641060031456</v>
       </c>
       <c r="F489" t="n">
-        <v>26.13073188415613</v>
+        <v>26.16459732584357</v>
       </c>
       <c r="G489" t="n">
-        <v>22.73591358165149</v>
+        <v>22.87167033771589</v>
       </c>
       <c r="H489" t="n">
-        <v>25.94516653229659</v>
+        <v>25.98351617428573</v>
       </c>
       <c r="I489" t="n">
-        <v>20.56065366950572</v>
+        <v>20.63057620252181</v>
       </c>
       <c r="J489" t="n">
-        <v>19.58947098380545</v>
+        <v>19.72481447822642</v>
       </c>
       <c r="K489" t="n">
-        <v>17.01366732388103</v>
+        <v>17.15029323535972</v>
       </c>
       <c r="L489" t="n">
-        <v>24.49224560113683</v>
+        <v>24.44900147591562</v>
       </c>
       <c r="M489" t="n">
-        <v>20.01325015506319</v>
+        <v>20.16550576555362</v>
       </c>
       <c r="N489" t="n">
-        <v>20.39389992015544</v>
+        <v>20.52985036874689</v>
       </c>
       <c r="O489" t="n">
-        <v>23.88215904377358</v>
+        <v>23.90296252045044</v>
       </c>
       <c r="P489" t="n">
-        <v>23.20471448450898</v>
+        <v>23.1297407006409</v>
       </c>
       <c r="Q489" t="n">
-        <v>19.08694153890807</v>
+        <v>19.15713693665029</v>
       </c>
       <c r="R489" t="n">
-        <v>25.47555058572471</v>
+        <v>25.47729624962837</v>
       </c>
       <c r="S489" t="n">
-        <v>19.67490532075106</v>
+        <v>19.82499703842862</v>
       </c>
       <c r="T489" t="n">
-        <v>21.15647999108166</v>
+        <v>21.23486273539116</v>
       </c>
       <c r="U489" t="n">
-        <v>25.63843847324503</v>
+        <v>25.68551799073718</v>
       </c>
       <c r="V489" t="n">
-        <v>27.06071326078566</v>
+        <v>27.03001699189422</v>
       </c>
       <c r="W489" t="n">
-        <v>21.37040744087335</v>
+        <v>21.4696548704495</v>
       </c>
       <c r="X489" t="n">
-        <v>17.24570163178509</v>
+        <v>17.36917835736494</v>
       </c>
       <c r="Y489" t="n">
-        <v>18.66101724865195</v>
+        <v>18.81638140630958</v>
       </c>
       <c r="Z489" t="n">
-        <v>14.48508929058997</v>
+        <v>14.61989135173244</v>
       </c>
       <c r="AA489" t="n">
-        <v>17.54101639293043</v>
+        <v>17.68571906714115</v>
       </c>
       <c r="AB489" t="n">
-        <v>17.78202360402159</v>
+        <v>17.89487862280343</v>
       </c>
       <c r="AC489" t="n">
-        <v>15.08481910956203</v>
+        <v>15.21427759001019</v>
       </c>
       <c r="AD489" t="n">
-        <v>16.13311726668886</v>
+        <v>16.25813079784398</v>
       </c>
       <c r="AE489" t="n">
-        <v>24.39310932390579</v>
+        <v>24.34820161936743</v>
       </c>
       <c r="AF489" t="n">
-        <v>22.17710255969773</v>
+        <v>22.29915005983986</v>
       </c>
       <c r="AG489" t="n">
-        <v>21.22334460052512</v>
+        <v>21.15638225640711</v>
       </c>
       <c r="AH489" t="n">
-        <v>25.73850673871966</v>
+        <v>25.70219518266232</v>
       </c>
       <c r="AI489" t="n">
-        <v>20.21397563421616</v>
+        <v>20.30063684044892</v>
       </c>
       <c r="AJ489" t="n">
-        <v>27.4669966368318</v>
+        <v>27.37304612518996</v>
       </c>
       <c r="AK489" t="n">
-        <v>17.82741112493899</v>
+        <v>17.94091166716937</v>
       </c>
       <c r="AL489" t="n">
-        <v>26.5114087776216</v>
+        <v>26.55363051545257</v>
       </c>
       <c r="AM489" t="n">
-        <v>22.48523149207128</v>
+        <v>22.48450564097381</v>
       </c>
     </row>
     <row r="490">
       <c r="A490" s="2" t="n">
-        <v>45535</v>
+        <v>45536</v>
       </c>
       <c r="B490" t="n">
-        <v>20.99357057158879</v>
+        <v>21.05881166582265</v>
       </c>
       <c r="C490" t="n">
-        <v>18.1238239022452</v>
+        <v>18.09300705464707</v>
       </c>
       <c r="D490" t="n">
-        <v>18.5568163181416</v>
+        <v>18.48566493111889</v>
       </c>
       <c r="E490" t="n">
-        <v>22.37301604172517</v>
+        <v>22.42849349585554</v>
       </c>
       <c r="F490" t="n">
-        <v>27.48900629267779</v>
+        <v>27.26732929685402</v>
       </c>
       <c r="G490" t="n">
-        <v>23.80888960925969</v>
+        <v>23.44437157896449</v>
       </c>
       <c r="H490" t="n">
-        <v>27.14686985775948</v>
+        <v>27.02352884839888</v>
       </c>
       <c r="I490" t="n">
-        <v>21.94134107444567</v>
+        <v>21.86966507399714</v>
       </c>
       <c r="J490" t="n">
-        <v>20.57700486198085</v>
+        <v>20.38739080408549</v>
       </c>
       <c r="K490" t="n">
-        <v>17.95760555970793</v>
+        <v>17.902968105576</v>
       </c>
       <c r="L490" t="n">
-        <v>25.31534943435989</v>
+        <v>25.23714786889254</v>
       </c>
       <c r="M490" t="n">
-        <v>21.15436490023663</v>
+        <v>20.91470079247798</v>
       </c>
       <c r="N490" t="n">
-        <v>21.46492317958957</v>
+        <v>21.19803768810081</v>
       </c>
       <c r="O490" t="n">
-        <v>25.09640437861875</v>
+        <v>25.02210165475548</v>
       </c>
       <c r="P490" t="n">
-        <v>24.18125923115743</v>
+        <v>24.04924912137458</v>
       </c>
       <c r="Q490" t="n">
-        <v>20.10713900314659</v>
+        <v>20.18229458446786</v>
       </c>
       <c r="R490" t="n">
-        <v>26.27628608928614</v>
+        <v>26.17035232911659</v>
       </c>
       <c r="S490" t="n">
-        <v>20.92647765977093</v>
+        <v>20.97343738735696</v>
       </c>
       <c r="T490" t="n">
-        <v>22.37358875209718</v>
+        <v>22.33389493448167</v>
       </c>
       <c r="U490" t="n">
-        <v>27.23227741318135</v>
+        <v>26.80422898677408</v>
       </c>
       <c r="V490" t="n">
-        <v>28.1569800040174</v>
+        <v>28.1435541435782</v>
       </c>
       <c r="W490" t="n">
-        <v>22.48007162684801</v>
+        <v>22.44353923627632</v>
       </c>
       <c r="X490" t="n">
-        <v>18.35492345438233</v>
+        <v>18.48549024780353</v>
       </c>
       <c r="Y490" t="n">
-        <v>19.90508096051274</v>
+        <v>19.95361880097787</v>
       </c>
       <c r="Z490" t="n">
-        <v>15.40386398868089</v>
+        <v>15.54651918785769</v>
       </c>
       <c r="AA490" t="n">
-        <v>18.48169158058375</v>
+        <v>18.43860546622465</v>
       </c>
       <c r="AB490" t="n">
-        <v>19.05869765827662</v>
+        <v>19.04185353792041</v>
       </c>
       <c r="AC490" t="n">
-        <v>15.99247038588382</v>
+        <v>16.14037463441355</v>
       </c>
       <c r="AD490" t="n">
-        <v>17.10594356567474</v>
+        <v>17.24901415518719</v>
       </c>
       <c r="AE490" t="n">
-        <v>25.33065468417066</v>
+        <v>25.3621266227924</v>
       </c>
       <c r="AF490" t="n">
-        <v>23.17358083046904</v>
+        <v>22.82282817499207</v>
       </c>
       <c r="AG490" t="n">
-        <v>22.38173881198946</v>
+        <v>22.30505274576677</v>
       </c>
       <c r="AH490" t="n">
-        <v>26.9010160737577</v>
+        <v>26.75301219245802</v>
       </c>
       <c r="AI490" t="n">
-        <v>21.33710730505328</v>
+        <v>21.3779906162479</v>
       </c>
       <c r="AJ490" t="n">
-        <v>28.61086169524685</v>
+        <v>28.53757307524634</v>
       </c>
       <c r="AK490" t="n">
-        <v>18.74458761803346</v>
+        <v>18.74158810416586</v>
       </c>
       <c r="AL490" t="n">
-        <v>28.08660069410164</v>
+        <v>27.67369322130919</v>
       </c>
       <c r="AM490" t="n">
-        <v>23.64301590851032</v>
+        <v>23.66438774114306</v>
       </c>
     </row>
     <row r="491">
       <c r="A491" s="2" t="n">
-        <v>45565</v>
+        <v>45566</v>
       </c>
       <c r="B491" t="n">
-        <v>21.41967049240261</v>
+        <v>21.35946805919921</v>
       </c>
       <c r="C491" t="n">
-        <v>18.81062250574881</v>
+        <v>18.61285019631536</v>
       </c>
       <c r="D491" t="n">
-        <v>18.69554742604462</v>
+        <v>18.59063505466966</v>
       </c>
       <c r="E491" t="n">
-        <v>23.01302363443191</v>
+        <v>23.0579203457931</v>
       </c>
       <c r="F491" t="n">
-        <v>28.1788924714352</v>
+        <v>28.31944692648489</v>
       </c>
       <c r="G491" t="n">
-        <v>23.58248715381487</v>
+        <v>23.59287347683261</v>
       </c>
       <c r="H491" t="n">
-        <v>27.37546762939168</v>
+        <v>27.65496867534919</v>
       </c>
       <c r="I491" t="n">
-        <v>22.49388854939884</v>
+        <v>22.62843051439443</v>
       </c>
       <c r="J491" t="n">
-        <v>20.70247977646243</v>
+        <v>20.63090732252208</v>
       </c>
       <c r="K491" t="n">
-        <v>18.36791265816991</v>
+        <v>18.2268834431882</v>
       </c>
       <c r="L491" t="n">
-        <v>26.06599451729026</v>
+        <v>26.29679122513988</v>
       </c>
       <c r="M491" t="n">
-        <v>21.42006112362807</v>
+        <v>21.29881069390182</v>
       </c>
       <c r="N491" t="n">
-        <v>21.57979907798907</v>
+        <v>21.50849788630352</v>
       </c>
       <c r="O491" t="n">
-        <v>25.61751289942312</v>
+        <v>25.78164244321224</v>
       </c>
       <c r="P491" t="n">
-        <v>24.96657817829587</v>
+        <v>25.27474419186534</v>
       </c>
       <c r="Q491" t="n">
-        <v>20.48787110565126</v>
+        <v>20.49882002282653</v>
       </c>
       <c r="R491" t="n">
-        <v>27.08643053473379</v>
+        <v>27.17618830605886</v>
       </c>
       <c r="S491" t="n">
-        <v>21.59982637758254</v>
+        <v>21.61927388830399</v>
       </c>
       <c r="T491" t="n">
-        <v>22.98767091493514</v>
+        <v>23.14890277686366</v>
       </c>
       <c r="U491" t="n">
-        <v>26.91482064345781</v>
+        <v>27.10066725353271</v>
       </c>
       <c r="V491" t="n">
-        <v>28.2184041328267</v>
+        <v>28.44325031435512</v>
       </c>
       <c r="W491" t="n">
-        <v>22.62790749783871</v>
+        <v>22.76817628406227</v>
       </c>
       <c r="X491" t="n">
-        <v>19.04027899684062</v>
+        <v>19.01044541927466</v>
       </c>
       <c r="Y491" t="n">
-        <v>20.5027674714022</v>
+        <v>20.51135458594324</v>
       </c>
       <c r="Z491" t="n">
-        <v>16.12951765069419</v>
+        <v>15.96475871151965</v>
       </c>
       <c r="AA491" t="n">
-        <v>18.74199378768113</v>
+        <v>18.64364273877408</v>
       </c>
       <c r="AB491" t="n">
-        <v>19.82263595185507</v>
+        <v>19.67931554830113</v>
       </c>
       <c r="AC491" t="n">
-        <v>16.70604600534701</v>
+        <v>16.49435984973211</v>
       </c>
       <c r="AD491" t="n">
-        <v>17.71107598864613</v>
+        <v>17.6467414990323</v>
       </c>
       <c r="AE491" t="n">
-        <v>25.45107256363015</v>
+        <v>25.63530538009137</v>
       </c>
       <c r="AF491" t="n">
-        <v>22.99927447286585</v>
+        <v>23.00809350360986</v>
       </c>
       <c r="AG491" t="n">
-        <v>23.2124445271626</v>
+        <v>23.54870586804563</v>
       </c>
       <c r="AH491" t="n">
-        <v>27.53399401042419</v>
+        <v>27.67951827206199</v>
       </c>
       <c r="AI491" t="n">
-        <v>21.76748147858035</v>
+        <v>21.82396221842275</v>
       </c>
       <c r="AJ491" t="n">
-        <v>28.63348937326649</v>
+        <v>28.66918797248328</v>
       </c>
       <c r="AK491" t="n">
-        <v>18.9249359958644</v>
+        <v>18.8376544168513</v>
       </c>
       <c r="AL491" t="n">
-        <v>28.13314025630704</v>
+        <v>28.44305810602719</v>
       </c>
       <c r="AM491" t="n">
-        <v>23.93610497491872</v>
+        <v>23.8772247290897</v>
       </c>
     </row>
     <row r="492">
       <c r="A492" s="2" t="n">
-        <v>45596</v>
+        <v>45597</v>
       </c>
       <c r="B492" t="n">
-        <v>20.6388516948886</v>
+        <v>20.6233259095292</v>
       </c>
       <c r="C492" t="n">
-        <v>18.27236501499334</v>
+        <v>18.49040806777504</v>
       </c>
       <c r="D492" t="n">
-        <v>18.43512261038299</v>
+        <v>18.3772323825328</v>
       </c>
       <c r="E492" t="n">
-        <v>22.25195037997398</v>
+        <v>22.25338477328405</v>
       </c>
       <c r="F492" t="n">
-        <v>27.93907918923999</v>
+        <v>28.13839081854881</v>
       </c>
       <c r="G492" t="n">
-        <v>22.69635821460036</v>
+        <v>22.88932462592012</v>
       </c>
       <c r="H492" t="n">
-        <v>26.55164104574298</v>
+        <v>26.50589892736611</v>
       </c>
       <c r="I492" t="n">
-        <v>22.04843560489285</v>
+        <v>22.05341338214321</v>
       </c>
       <c r="J492" t="n">
-        <v>20.34210511487833</v>
+        <v>20.42453863648038</v>
       </c>
       <c r="K492" t="n">
-        <v>17.86617513405453</v>
+        <v>18.01101367845606</v>
       </c>
       <c r="L492" t="n">
-        <v>26.56828100817899</v>
+        <v>26.82401261553932</v>
       </c>
       <c r="M492" t="n">
-        <v>20.62063436679935</v>
+        <v>20.87341799528306</v>
       </c>
       <c r="N492" t="n">
-        <v>20.95307126432747</v>
+        <v>21.20071290407651</v>
       </c>
       <c r="O492" t="n">
-        <v>25.08787054004</v>
+        <v>25.17489837812168</v>
       </c>
       <c r="P492" t="n">
-        <v>25.61002916687577</v>
+        <v>25.87927039544163</v>
       </c>
       <c r="Q492" t="n">
-        <v>19.61617500665213</v>
+        <v>19.52278617600588</v>
       </c>
       <c r="R492" t="n">
-        <v>27.55778436022164</v>
+        <v>27.82196925030758</v>
       </c>
       <c r="S492" t="n">
-        <v>21.04331811228756</v>
+        <v>20.98026276075265</v>
       </c>
       <c r="T492" t="n">
-        <v>22.74864597666717</v>
+        <v>22.74604655536175</v>
       </c>
       <c r="U492" t="n">
-        <v>26.02174184454257</v>
+        <v>26.11051413517125</v>
       </c>
       <c r="V492" t="n">
-        <v>27.479710197526</v>
+        <v>27.49141247348539</v>
       </c>
       <c r="W492" t="n">
-        <v>21.66098083249814</v>
+        <v>21.6120676862617</v>
       </c>
       <c r="X492" t="n">
-        <v>18.53564879850233</v>
+        <v>18.51047094212076</v>
       </c>
       <c r="Y492" t="n">
-        <v>19.88026668186134</v>
+        <v>19.84083099170747</v>
       </c>
       <c r="Z492" t="n">
-        <v>15.8267268322269</v>
+        <v>15.86453965425851</v>
       </c>
       <c r="AA492" t="n">
-        <v>18.29582833301164</v>
+        <v>18.30480704945037</v>
       </c>
       <c r="AB492" t="n">
-        <v>19.29751623951341</v>
+        <v>19.4033957046308</v>
       </c>
       <c r="AC492" t="n">
-        <v>16.25977999550249</v>
+        <v>16.3019230436457</v>
       </c>
       <c r="AD492" t="n">
-        <v>17.20627205482614</v>
+        <v>17.17777339026696</v>
       </c>
       <c r="AE492" t="n">
-        <v>24.44694054998095</v>
+        <v>24.37325312458867</v>
       </c>
       <c r="AF492" t="n">
-        <v>22.55345962842024</v>
+        <v>22.7078492093909</v>
       </c>
       <c r="AG492" t="n">
-        <v>23.62183407194634</v>
+        <v>23.82292984047158</v>
       </c>
       <c r="AH492" t="n">
-        <v>27.28742919251476</v>
+        <v>27.56680080714363</v>
       </c>
       <c r="AI492" t="n">
-        <v>20.89209420266547</v>
+        <v>20.89094771771106</v>
       </c>
       <c r="AJ492" t="n">
-        <v>27.73712216951745</v>
+        <v>27.79191159284686</v>
       </c>
       <c r="AK492" t="n">
-        <v>18.4294315141569</v>
+        <v>18.38788232273468</v>
       </c>
       <c r="AL492" t="n">
-        <v>27.5146386462453</v>
+        <v>27.54635991779716</v>
       </c>
       <c r="AM492" t="n">
-        <v>23.10120082605821</v>
+        <v>23.06306788389408</v>
       </c>
     </row>
     <row r="493">
       <c r="A493" s="2" t="n">
-        <v>45626</v>
+        <v>45627</v>
       </c>
       <c r="B493" t="n">
-        <v>20.1850975032347</v>
+        <v>20.53132850839767</v>
       </c>
       <c r="C493" t="n">
-        <v>18.2807945713391</v>
+        <v>18.67961911323902</v>
       </c>
       <c r="D493" t="n">
-        <v>18.14566121638508</v>
+        <v>18.46216100126412</v>
       </c>
       <c r="E493" t="n">
-        <v>22.04695287018079</v>
+        <v>22.13330677015334</v>
       </c>
       <c r="F493" t="n">
-        <v>28.24233451463294</v>
+        <v>28.52306734433104</v>
       </c>
       <c r="G493" t="n">
-        <v>22.65690873487956</v>
+        <v>23.17959112401362</v>
       </c>
       <c r="H493" t="n">
-        <v>26.19910608862988</v>
+        <v>26.48624605160636</v>
       </c>
       <c r="I493" t="n">
-        <v>21.67935782539602</v>
+        <v>21.80898139980876</v>
       </c>
       <c r="J493" t="n">
-        <v>20.20016904325894</v>
+        <v>20.60279720703246</v>
       </c>
       <c r="K493" t="n">
-        <v>17.68800242334227</v>
+        <v>18.02825807519874</v>
       </c>
       <c r="L493" t="n">
-        <v>27.2663150101176</v>
+        <v>27.10082157411101</v>
       </c>
       <c r="M493" t="n">
-        <v>20.56767757405495</v>
+        <v>21.04501407852809</v>
       </c>
       <c r="N493" t="n">
-        <v>20.94165513303578</v>
+        <v>21.41337135404527</v>
       </c>
       <c r="O493" t="n">
-        <v>25.25069855157513</v>
+        <v>25.35552054991506</v>
       </c>
       <c r="P493" t="n">
-        <v>26.38923537762509</v>
+        <v>26.2122633592287</v>
       </c>
       <c r="Q493" t="n">
-        <v>18.85856649089372</v>
+        <v>19.06863716192744</v>
       </c>
       <c r="R493" t="n">
-        <v>28.04593962986669</v>
+        <v>28.0970097250955</v>
       </c>
       <c r="S493" t="n">
-        <v>20.57461077422149</v>
+        <v>20.71672434759211</v>
       </c>
       <c r="T493" t="n">
-        <v>22.52594185694871</v>
+        <v>22.54810862362479</v>
       </c>
       <c r="U493" t="n">
-        <v>25.6070085565939</v>
+        <v>26.17855482509945</v>
       </c>
       <c r="V493" t="n">
-        <v>27.27689549997525</v>
+        <v>27.82419020938066</v>
       </c>
       <c r="W493" t="n">
-        <v>21.16990584454134</v>
+        <v>21.32761947827793</v>
       </c>
       <c r="X493" t="n">
-        <v>18.18463818713327</v>
+        <v>18.29885925725259</v>
       </c>
       <c r="Y493" t="n">
-        <v>19.45566911405923</v>
+        <v>19.63309053276197</v>
       </c>
       <c r="Z493" t="n">
-        <v>15.61707326400327</v>
+        <v>15.88794701443229</v>
       </c>
       <c r="AA493" t="n">
-        <v>17.96586815178751</v>
+        <v>18.2942234683051</v>
       </c>
       <c r="AB493" t="n">
-        <v>19.12710441253902</v>
+        <v>19.54233413337477</v>
       </c>
       <c r="AC493" t="n">
-        <v>15.96437111244156</v>
+        <v>16.23428331825674</v>
       </c>
       <c r="AD493" t="n">
-        <v>16.76846809689954</v>
+        <v>16.88704921374656</v>
       </c>
       <c r="AE493" t="n">
-        <v>23.88179028674627</v>
+        <v>24.1465595691846</v>
       </c>
       <c r="AF493" t="n">
-        <v>22.61237682816846</v>
+        <v>23.14771055740579</v>
       </c>
       <c r="AG493" t="n">
-        <v>23.95783773703597</v>
+        <v>23.76816559649749</v>
       </c>
       <c r="AH493" t="n">
-        <v>27.94721800427128</v>
+        <v>28.10781775592589</v>
       </c>
       <c r="AI493" t="n">
-        <v>20.58647977252118</v>
+        <v>20.66924611604349</v>
       </c>
       <c r="AJ493" t="n">
-        <v>27.35697245153538</v>
+        <v>28.04319675156979</v>
       </c>
       <c r="AK493" t="n">
-        <v>18.07153898327787</v>
+        <v>18.3998025732325</v>
       </c>
       <c r="AL493" t="n">
-        <v>27.27376904328503</v>
+        <v>27.79864174047745</v>
       </c>
       <c r="AM493" t="n">
-        <v>22.71990366009032</v>
+        <v>23.20395702049265</v>
       </c>
     </row>
   </sheetData>

</xml_diff>